<commit_message>
Solved bug SDTR=0 when amt2reduce > 0
</commit_message>
<xml_diff>
--- a/DRP/demand_data.xlsx
+++ b/DRP/demand_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21A7592-F3B8-42AE-815D-089914A8E924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D8632-7A78-4827-AD88-768A4F03CABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="960" windowWidth="21408" windowHeight="11652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21375" yWindow="2355" windowWidth="17280" windowHeight="8970" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="134">
   <si>
     <t>W46</t>
   </si>
@@ -518,9 +518,6 @@
   </si>
   <si>
     <t>Original</t>
-  </si>
-  <si>
-    <t>STDR (accum)</t>
   </si>
   <si>
     <t>SDTR (accum)</t>
@@ -3875,7 +3872,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4140,7 +4137,7 @@
         <v>15</v>
       </c>
       <c r="I13" s="11">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="J13" s="11">
         <v>0</v>
@@ -4312,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9570860C-3C86-4334-8A6D-B1198D355506}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4578,7 +4575,7 @@
         <v>15</v>
       </c>
       <c r="I13" s="11">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="J13" s="11">
         <v>10</v>
@@ -4742,8 +4739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C51A3B-D959-48BB-8764-4DF003928E26}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5008,7 +5005,7 @@
       </c>
       <c r="H13" s="217"/>
       <c r="I13" s="217">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="J13" s="217">
         <v>15</v>
@@ -5179,7 +5176,7 @@
   <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5356,8 +5353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B409AB02-E9CA-40CB-B386-70D450CE0A6B}">
   <dimension ref="A2:AH209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R126" sqref="R126"/>
+    <sheetView tabSelected="1" topLeftCell="D108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M140" sqref="M140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5594,7 +5591,7 @@
       </c>
       <c r="L14" s="256">
         <f>'DC1'!I13</f>
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="M14" s="256">
         <f>'DC1'!J13</f>
@@ -5787,7 +5784,7 @@
       </c>
       <c r="L18" s="63">
         <f t="shared" si="0"/>
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="M18" s="63">
         <f t="shared" si="0"/>
@@ -5861,19 +5858,19 @@
       </c>
       <c r="L20" s="70">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="M20" s="70">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="N20" s="70">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O20" s="71">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="Q20" s="72" t="s">
         <v>50</v>
@@ -5913,7 +5910,7 @@
       </c>
       <c r="L21" s="199">
         <f t="shared" si="3"/>
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="M21" s="199">
         <f t="shared" si="3"/>
@@ -5921,11 +5918,11 @@
       </c>
       <c r="N21" s="199">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="O21" s="279">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q21" s="72" t="s">
         <v>53</v>
@@ -5956,7 +5953,7 @@
       </c>
       <c r="L22" s="70">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="M22" s="70">
         <f t="shared" si="4"/>
@@ -5994,7 +5991,7 @@
       </c>
       <c r="J23" s="77">
         <f t="shared" si="5"/>
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="K23" s="77">
         <f t="shared" si="5"/>
@@ -6040,7 +6037,7 @@
       </c>
       <c r="J24" s="81">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="81">
         <f t="shared" si="6"/>
@@ -6087,7 +6084,7 @@
       </c>
       <c r="J25" s="85">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K25" s="85">
         <f t="shared" si="7"/>
@@ -6133,7 +6130,7 @@
       </c>
       <c r="J26" s="89">
         <f t="shared" si="8"/>
-        <v>4800</v>
+        <v>5750</v>
       </c>
       <c r="K26" s="89">
         <f t="shared" si="8"/>
@@ -6228,7 +6225,7 @@
       </c>
       <c r="J28" s="98">
         <f t="shared" si="9"/>
-        <v>34400</v>
+        <v>40850</v>
       </c>
       <c r="K28" s="98">
         <f t="shared" si="9"/>
@@ -6280,7 +6277,7 @@
       </c>
       <c r="J29" s="102">
         <f t="shared" si="10"/>
-        <v>39200</v>
+        <v>46600</v>
       </c>
       <c r="K29" s="102">
         <f t="shared" si="10"/>
@@ -6378,7 +6375,7 @@
       </c>
       <c r="J31" s="106">
         <f t="shared" si="11"/>
-        <v>66880</v>
+        <v>79420</v>
       </c>
       <c r="K31" s="106">
         <f t="shared" si="11"/>
@@ -6427,7 +6424,7 @@
       </c>
       <c r="J32" s="110">
         <f t="shared" si="12"/>
-        <v>27680</v>
+        <v>32820</v>
       </c>
       <c r="K32" s="110">
         <f t="shared" si="12"/>
@@ -6476,7 +6473,7 @@
       </c>
       <c r="J33" s="81">
         <f t="shared" si="13"/>
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="K33" s="81">
         <f t="shared" si="13"/>
@@ -6535,7 +6532,7 @@
       </c>
       <c r="J34" s="81">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K34" s="81">
         <f t="shared" si="14"/>
@@ -6565,7 +6562,7 @@
     </row>
     <row r="35" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D35" s="278" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E35" s="273"/>
       <c r="F35" s="274">
@@ -6586,7 +6583,7 @@
       </c>
       <c r="J35" s="274">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K35" s="274">
         <f t="shared" si="15"/>
@@ -6604,9 +6601,8 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="O35" s="274" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
+      <c r="O35" s="275">
+        <v>0</v>
       </c>
       <c r="P35" s="50"/>
       <c r="AC35" s="117"/>
@@ -6637,7 +6633,7 @@
       </c>
       <c r="J36" s="85">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="85">
         <f t="shared" si="16"/>
@@ -6710,7 +6706,7 @@
       </c>
       <c r="J37" s="85">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="85">
         <f t="shared" si="17"/>
@@ -6804,7 +6800,7 @@
       </c>
       <c r="J38" s="132">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="K38" s="132">
         <f t="shared" si="18"/>
@@ -6882,45 +6878,45 @@
       <c r="D39" s="135" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="96"/>
-      <c r="F39" s="97">
-        <f>F34*F27</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="97">
-        <f t="shared" ref="G39:O39" si="27">G34*G27</f>
-        <v>0</v>
-      </c>
-      <c r="H39" s="97">
+      <c r="E39" s="92"/>
+      <c r="F39" s="140">
+        <f t="shared" ref="F39:I39" si="27">F35*F27</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="140">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="I39" s="97">
+      <c r="H39" s="140">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="J39" s="97">
+      <c r="I39" s="140">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="K39" s="97">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="L39" s="97">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="97">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="N39" s="97">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="O39" s="136">
-        <f t="shared" si="27"/>
+      <c r="J39" s="140">
+        <f>J35*J27</f>
+        <v>5375</v>
+      </c>
+      <c r="K39" s="140">
+        <f t="shared" ref="K39:O39" si="28">K35*K27</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="140">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="M39" s="140">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="140">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="141">
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="P39" s="134"/>
@@ -6983,39 +6979,39 @@
         <v>0</v>
       </c>
       <c r="G40" s="110">
-        <f t="shared" ref="G40:O40" si="28">G39+G38</f>
+        <f t="shared" ref="G40:O40" si="29">G39+G38</f>
         <v>0</v>
       </c>
       <c r="H40" s="110">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="I40" s="110">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="J40" s="110">
-        <f t="shared" si="28"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>6325</v>
       </c>
       <c r="K40" s="110">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L40" s="110">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="M40" s="110">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="N40" s="110">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="O40" s="111">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="P40" s="58"/>
@@ -7073,43 +7069,43 @@
       </c>
       <c r="E41" s="92"/>
       <c r="F41" s="140">
-        <f>F34*F30</f>
+        <f t="shared" ref="F41:I41" si="30">F35*F30</f>
         <v>0</v>
       </c>
       <c r="G41" s="140">
-        <f t="shared" ref="G41:O41" si="29">G34*G30</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="H41" s="140">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="I41" s="140">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="J41" s="140">
-        <f t="shared" si="29"/>
-        <v>0</v>
+        <f>J35*J30</f>
+        <v>10450</v>
       </c>
       <c r="K41" s="140">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="K41:O41" si="31">K35*K30</f>
         <v>0</v>
       </c>
       <c r="L41" s="140">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="M41" s="140">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="N41" s="140">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="O41" s="141">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P41" s="58"/>
@@ -7175,35 +7171,35 @@
         <v>0</v>
       </c>
       <c r="H42" s="144">
-        <f t="shared" ref="H42:O42" si="30">H41-H40</f>
+        <f t="shared" ref="H42:O42" si="32">H41-H40</f>
         <v>0</v>
       </c>
       <c r="I42" s="143">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J42" s="143">
-        <f t="shared" si="30"/>
-        <v>0</v>
+        <f t="shared" si="32"/>
+        <v>4125</v>
       </c>
       <c r="K42" s="143">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="L42" s="143">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="M42" s="143">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="N42" s="143">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="O42" s="145">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="P42" s="50" t="s">
@@ -7271,35 +7267,35 @@
         <v>13760</v>
       </c>
       <c r="H43" s="148">
-        <f t="shared" ref="H43:O43" si="31">H32-H42</f>
+        <f t="shared" ref="H43:O43" si="33">H32-H42</f>
         <v>16700</v>
       </c>
       <c r="I43" s="148">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>3400</v>
       </c>
       <c r="J43" s="148">
-        <f t="shared" si="31"/>
-        <v>27680</v>
+        <f t="shared" si="33"/>
+        <v>28695</v>
       </c>
       <c r="K43" s="148">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="L43" s="148">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>7160</v>
       </c>
       <c r="M43" s="148">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1720</v>
       </c>
       <c r="N43" s="148">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="O43" s="149">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V43">
@@ -7360,39 +7356,39 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G44" s="152">
-        <f t="shared" ref="G44:O44" si="32">G33/G23</f>
+        <f t="shared" ref="G44:O44" si="34">G33/G23</f>
         <v>0.375</v>
       </c>
       <c r="H44" s="152">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.4</v>
       </c>
       <c r="I44" s="152">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0.75</v>
       </c>
       <c r="J44" s="152">
-        <f t="shared" si="32"/>
-        <v>0.78125</v>
+        <f t="shared" si="34"/>
+        <v>0.78947368421052633</v>
       </c>
       <c r="K44" s="152" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L44" s="152">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M44" s="152">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="N44" s="152" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O44" s="152" t="e">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V44">
@@ -7453,39 +7449,39 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G45" s="152">
-        <f t="shared" ref="G45:O45" si="33">G40/G29</f>
+        <f t="shared" ref="G45:O45" si="35">G40/G29</f>
         <v>0</v>
       </c>
       <c r="H45" s="152">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="I45" s="152">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J45" s="152">
-        <f t="shared" si="33"/>
-        <v>0</v>
+        <f t="shared" si="35"/>
+        <v>0.13572961373390557</v>
       </c>
       <c r="K45" s="152" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L45" s="152">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="M45" s="152">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="N45" s="152" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O45" s="152" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V45">
@@ -7546,39 +7542,39 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G46" s="152">
-        <f t="shared" ref="G46:O46" si="34">G42/G32</f>
+        <f t="shared" ref="G46:O46" si="36">G42/G32</f>
         <v>0</v>
       </c>
       <c r="H46" s="152">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="I46" s="152">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J46" s="152">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>0.1256855575868373</v>
       </c>
       <c r="K46" s="152" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L46" s="152">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="M46" s="152">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="N46" s="152" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O46" s="152" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V46">
@@ -8241,7 +8237,7 @@
       </c>
       <c r="L58" s="256">
         <f>'DC2'!I13</f>
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="M58" s="256">
         <f>'DC2'!J13</f>
@@ -8592,35 +8588,35 @@
         <v>0</v>
       </c>
       <c r="G62" s="63">
-        <f t="shared" ref="G62:N62" si="35">SUM(G58:G61)</f>
+        <f t="shared" ref="G62:N62" si="37">SUM(G58:G61)</f>
         <v>50</v>
       </c>
       <c r="H62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="I62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>80</v>
       </c>
       <c r="J62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>100</v>
       </c>
       <c r="K62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>15</v>
       </c>
       <c r="L62" s="63">
-        <f t="shared" si="35"/>
-        <v>185</v>
+        <f t="shared" si="37"/>
+        <v>190</v>
       </c>
       <c r="M62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="N62" s="63">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>50</v>
       </c>
       <c r="O62" s="64">
@@ -8757,40 +8753,40 @@
         <v>50</v>
       </c>
       <c r="G64" s="70">
-        <f t="shared" ref="G64:O64" si="36">F64+G63+G66-G62</f>
+        <f t="shared" ref="G64:O64" si="38">F64+G63+G66-G62</f>
         <v>20</v>
       </c>
       <c r="H64" s="70">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>20</v>
       </c>
       <c r="I64" s="70">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>20</v>
       </c>
       <c r="J64" s="70">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>20</v>
       </c>
       <c r="K64" s="70">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>25</v>
       </c>
       <c r="L64" s="70">
-        <f t="shared" si="36"/>
-        <v>20</v>
+        <f t="shared" si="38"/>
+        <v>35</v>
       </c>
       <c r="M64" s="70">
-        <f t="shared" si="36"/>
-        <v>30</v>
+        <f t="shared" si="38"/>
+        <v>25</v>
       </c>
       <c r="N64" s="70">
-        <f t="shared" si="36"/>
-        <v>20</v>
+        <f t="shared" si="38"/>
+        <v>35</v>
       </c>
       <c r="O64" s="71">
-        <f t="shared" si="36"/>
-        <v>30</v>
+        <f t="shared" si="38"/>
+        <v>25</v>
       </c>
       <c r="Q64" s="72" t="s">
         <v>50</v>
@@ -8856,40 +8852,40 @@
         <v>0</v>
       </c>
       <c r="G65" s="70">
-        <f t="shared" ref="G65:O65" si="37">IF(F64-G62&lt;=$E$56, G62-F64+$E$56,0)</f>
+        <f t="shared" ref="G65:O65" si="39">IF(F64-G62&lt;=$E$56, G62-F64+$E$56,0)</f>
         <v>20</v>
       </c>
       <c r="H65" s="70">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="I65" s="70">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>80</v>
       </c>
       <c r="J65" s="70">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>100</v>
       </c>
       <c r="K65" s="70">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>15</v>
       </c>
       <c r="L65" s="70">
-        <f t="shared" si="37"/>
-        <v>180</v>
+        <f t="shared" si="39"/>
+        <v>185</v>
       </c>
       <c r="M65" s="70">
-        <f t="shared" si="37"/>
-        <v>10</v>
+        <f t="shared" si="39"/>
+        <v>0</v>
       </c>
       <c r="N65" s="70">
-        <f t="shared" si="37"/>
-        <v>40</v>
+        <f t="shared" si="39"/>
+        <v>45</v>
       </c>
       <c r="O65" s="71">
-        <f t="shared" si="37"/>
-        <v>10</v>
+        <f t="shared" si="39"/>
+        <v>0</v>
       </c>
       <c r="Q65" s="72" t="s">
         <v>53</v>
@@ -8952,40 +8948,40 @@
         <v>0</v>
       </c>
       <c r="G66" s="70">
-        <f t="shared" ref="G66:O66" si="38" xml:space="preserve"> CEILING(G65/$E$55,1)*$E$55</f>
+        <f t="shared" ref="G66:O66" si="40" xml:space="preserve"> CEILING(G65/$E$55,1)*$E$55</f>
         <v>20</v>
       </c>
       <c r="H66" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="I66" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>80</v>
       </c>
       <c r="J66" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>100</v>
       </c>
       <c r="K66" s="70">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v>20</v>
       </c>
       <c r="L66" s="70">
-        <f t="shared" si="38"/>
-        <v>180</v>
+        <f t="shared" si="40"/>
+        <v>200</v>
       </c>
       <c r="M66" s="70">
-        <f t="shared" si="38"/>
-        <v>20</v>
+        <f t="shared" si="40"/>
+        <v>0</v>
       </c>
       <c r="N66" s="70">
-        <f t="shared" si="38"/>
-        <v>40</v>
+        <f t="shared" si="40"/>
+        <v>60</v>
       </c>
       <c r="O66" s="71">
-        <f t="shared" si="38"/>
-        <v>20</v>
+        <f t="shared" si="40"/>
+        <v>0</v>
       </c>
       <c r="V66">
         <f t="shared" si="19"/>
@@ -9045,39 +9041,39 @@
         <v>20</v>
       </c>
       <c r="G67" s="77">
-        <f t="shared" ref="G67:O67" si="39">H66</f>
+        <f t="shared" ref="G67:O67" si="41">H66</f>
         <v>0</v>
       </c>
       <c r="H67" s="77">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>80</v>
       </c>
       <c r="I67" s="77">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>100</v>
       </c>
       <c r="J67" s="77">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>20</v>
       </c>
       <c r="K67" s="77">
-        <f t="shared" si="39"/>
-        <v>180</v>
+        <f t="shared" si="41"/>
+        <v>200</v>
       </c>
       <c r="L67" s="77">
-        <f t="shared" si="39"/>
-        <v>20</v>
+        <f t="shared" si="41"/>
+        <v>0</v>
       </c>
       <c r="M67" s="77">
-        <f t="shared" si="39"/>
-        <v>40</v>
+        <f t="shared" si="41"/>
+        <v>60</v>
       </c>
       <c r="N67" s="77">
-        <f t="shared" si="39"/>
-        <v>20</v>
+        <f t="shared" si="41"/>
+        <v>0</v>
       </c>
       <c r="O67" s="78">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W67">
@@ -9134,39 +9130,39 @@
         <v>0</v>
       </c>
       <c r="G68" s="81">
-        <f t="shared" ref="G68:O68" si="40">QUOTIENT(MOD(G67+$E$50-1,$E$49),$E$50)</f>
+        <f t="shared" ref="G68:O68" si="42">QUOTIENT(MOD(G67+$E$50-1,$E$49),$E$50)</f>
         <v>0</v>
       </c>
       <c r="H68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="I68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="K68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="L68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="M68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="N68" s="81">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O68" s="82">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="W68">
@@ -9224,39 +9220,39 @@
         <v>1</v>
       </c>
       <c r="G69" s="85">
-        <f t="shared" ref="G69:O69" si="41">QUOTIENT(G67+$E$50-1,$E$49)</f>
+        <f t="shared" ref="G69:O69" si="43">QUOTIENT(G67+$E$50-1,$E$49)</f>
         <v>0</v>
       </c>
       <c r="H69" s="85">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>4</v>
       </c>
       <c r="I69" s="85">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>5</v>
       </c>
       <c r="J69" s="85">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="K69" s="85">
-        <f t="shared" si="41"/>
-        <v>9</v>
+        <f t="shared" si="43"/>
+        <v>10</v>
       </c>
       <c r="L69" s="85">
-        <f t="shared" si="41"/>
-        <v>1</v>
+        <f t="shared" si="43"/>
+        <v>0</v>
       </c>
       <c r="M69" s="85">
-        <f t="shared" si="41"/>
-        <v>2</v>
+        <f t="shared" si="43"/>
+        <v>3</v>
       </c>
       <c r="N69" s="85">
-        <f t="shared" si="41"/>
-        <v>1</v>
+        <f t="shared" si="43"/>
+        <v>0</v>
       </c>
       <c r="O69" s="86">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="W69">
@@ -9313,39 +9309,39 @@
         <v>500</v>
       </c>
       <c r="G70" s="89">
-        <f t="shared" ref="G70:O70" si="42">G69*$F$49+G68*$F$50</f>
+        <f t="shared" ref="G70:O70" si="44">G69*$F$49+G68*$F$50</f>
         <v>0</v>
       </c>
       <c r="H70" s="89">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>2000</v>
       </c>
       <c r="I70" s="89">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>2500</v>
       </c>
       <c r="J70" s="89">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>500</v>
       </c>
       <c r="K70" s="89">
-        <f t="shared" si="42"/>
-        <v>4500</v>
+        <f t="shared" si="44"/>
+        <v>5000</v>
       </c>
       <c r="L70" s="89">
-        <f t="shared" si="42"/>
-        <v>500</v>
+        <f t="shared" si="44"/>
+        <v>0</v>
       </c>
       <c r="M70" s="89">
-        <f t="shared" si="42"/>
-        <v>1000</v>
+        <f t="shared" si="44"/>
+        <v>1500</v>
       </c>
       <c r="N70" s="89">
-        <f t="shared" si="42"/>
-        <v>500</v>
+        <f t="shared" si="44"/>
+        <v>0</v>
       </c>
       <c r="O70" s="90">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="W70">
@@ -9490,43 +9486,43 @@
       </c>
       <c r="E72" s="96"/>
       <c r="F72" s="97">
-        <f t="shared" ref="F72:O72" si="43">F71*F67</f>
+        <f t="shared" ref="F72:O72" si="45">F71*F67</f>
         <v>4200</v>
       </c>
       <c r="G72" s="97">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="H72" s="97">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>17040</v>
       </c>
       <c r="I72" s="97">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>21500</v>
       </c>
       <c r="J72" s="97">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>4300</v>
       </c>
       <c r="K72" s="97">
-        <f t="shared" si="43"/>
-        <v>38880</v>
+        <f t="shared" si="45"/>
+        <v>43200</v>
       </c>
       <c r="L72" s="97">
-        <f t="shared" si="43"/>
-        <v>4280</v>
+        <f t="shared" si="45"/>
+        <v>0</v>
       </c>
       <c r="M72" s="97">
-        <f t="shared" si="43"/>
-        <v>8480</v>
+        <f t="shared" si="45"/>
+        <v>12720</v>
       </c>
       <c r="N72" s="97">
-        <f t="shared" si="43"/>
-        <v>4200</v>
+        <f t="shared" si="45"/>
+        <v>0</v>
       </c>
       <c r="O72" s="136">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="P72" s="50" t="s">
@@ -9582,43 +9578,43 @@
       </c>
       <c r="E73" s="101"/>
       <c r="F73" s="102">
-        <f t="shared" ref="F73:O73" si="44">F70+F72</f>
+        <f t="shared" ref="F73:O73" si="46">F70+F72</f>
         <v>4700</v>
       </c>
       <c r="G73" s="102">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="H73" s="102">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>19040</v>
       </c>
       <c r="I73" s="102">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>24000</v>
       </c>
       <c r="J73" s="102">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>4800</v>
       </c>
       <c r="K73" s="102">
-        <f t="shared" si="44"/>
-        <v>43380</v>
+        <f t="shared" si="46"/>
+        <v>48200</v>
       </c>
       <c r="L73" s="102">
-        <f t="shared" si="44"/>
-        <v>4780</v>
+        <f t="shared" si="46"/>
+        <v>0</v>
       </c>
       <c r="M73" s="102">
-        <f t="shared" si="44"/>
-        <v>9480</v>
+        <f t="shared" si="46"/>
+        <v>14220</v>
       </c>
       <c r="N73" s="102">
-        <f t="shared" si="44"/>
-        <v>4700</v>
+        <f t="shared" si="46"/>
+        <v>0</v>
       </c>
       <c r="O73" s="103">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P73" s="50" t="s">
@@ -9767,39 +9763,39 @@
         <v>8220</v>
       </c>
       <c r="G75" s="106">
-        <f t="shared" ref="G75:O75" si="45">G74*G67</f>
+        <f t="shared" ref="G75:O75" si="47">G74*G67</f>
         <v>0</v>
       </c>
       <c r="H75" s="106">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>32960</v>
       </c>
       <c r="I75" s="106">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>41300</v>
       </c>
       <c r="J75" s="106">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>8360</v>
       </c>
       <c r="K75" s="106">
-        <f t="shared" si="45"/>
-        <v>77040</v>
+        <f t="shared" si="47"/>
+        <v>85600</v>
       </c>
       <c r="L75" s="106">
-        <f t="shared" si="45"/>
-        <v>8520</v>
+        <f t="shared" si="47"/>
+        <v>0</v>
       </c>
       <c r="M75" s="106">
-        <f t="shared" si="45"/>
-        <v>16760</v>
+        <f t="shared" si="47"/>
+        <v>25140</v>
       </c>
       <c r="N75" s="106">
-        <f t="shared" si="45"/>
-        <v>8300</v>
+        <f t="shared" si="47"/>
+        <v>0</v>
       </c>
       <c r="O75" s="107">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="P75" s="50" t="s">
@@ -9859,39 +9855,39 @@
         <v>3520</v>
       </c>
       <c r="G76" s="110">
-        <f t="shared" ref="G76:O76" si="46">G75-G73</f>
+        <f t="shared" ref="G76:O76" si="48">G75-G73</f>
         <v>0</v>
       </c>
       <c r="H76" s="110">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>13920</v>
       </c>
       <c r="I76" s="110">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>17300</v>
       </c>
       <c r="J76" s="110">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>3560</v>
       </c>
       <c r="K76" s="110">
-        <f t="shared" si="46"/>
-        <v>33660</v>
+        <f t="shared" si="48"/>
+        <v>37400</v>
       </c>
       <c r="L76" s="110">
-        <f t="shared" si="46"/>
-        <v>3740</v>
+        <f t="shared" si="48"/>
+        <v>0</v>
       </c>
       <c r="M76" s="110">
-        <f t="shared" si="46"/>
-        <v>7280</v>
+        <f t="shared" si="48"/>
+        <v>10920</v>
       </c>
       <c r="N76" s="110">
-        <f t="shared" si="46"/>
-        <v>3600</v>
+        <f t="shared" si="48"/>
+        <v>0</v>
       </c>
       <c r="O76" s="111">
-        <f t="shared" si="46"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="P76" s="50" t="s">
@@ -9951,39 +9947,39 @@
         <v>10</v>
       </c>
       <c r="G77" s="223">
-        <f t="shared" ref="G77:O77" si="47">SUM(H58:H59)</f>
+        <f t="shared" ref="G77:O77" si="49">SUM(H58:H59)</f>
         <v>0</v>
       </c>
       <c r="H77" s="223">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>20</v>
       </c>
       <c r="I77" s="223">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>20</v>
       </c>
       <c r="J77" s="223">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>15</v>
       </c>
       <c r="K77" s="223">
-        <f t="shared" si="47"/>
-        <v>145</v>
+        <f t="shared" si="49"/>
+        <v>150</v>
       </c>
       <c r="L77" s="223">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>10</v>
       </c>
       <c r="M77" s="223">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="N77" s="223">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>10</v>
       </c>
       <c r="O77" s="224">
-        <f t="shared" si="47"/>
+        <f t="shared" si="49"/>
         <v>0</v>
       </c>
       <c r="P77" s="50" t="s">
@@ -10039,43 +10035,43 @@
       </c>
       <c r="E78" s="112"/>
       <c r="F78" s="81">
-        <f t="shared" ref="F78:O78" si="48">MIN(F151,F77)</f>
+        <f t="shared" ref="F78:O78" si="50">MIN(F151,F77)</f>
         <v>0</v>
       </c>
       <c r="G78" s="81">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="H78" s="81">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="I78" s="81">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="J78" s="81">
-        <f t="shared" si="48"/>
-        <v>0</v>
+        <f t="shared" si="50"/>
+        <v>15</v>
       </c>
       <c r="K78" s="81">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="L78" s="81">
-        <f t="shared" si="48"/>
-        <v>0</v>
+        <f t="shared" si="50"/>
+        <v>10</v>
       </c>
       <c r="M78" s="81">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="N78" s="81">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="O78" s="82">
-        <f t="shared" si="48"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="P78" s="50" t="s">
@@ -10131,44 +10127,44 @@
       </c>
       <c r="E79" s="273"/>
       <c r="F79" s="274">
-        <f>MIN(MAX(F$151-(H66-H65),0),F77)</f>
+        <f t="shared" ref="F79:I79" si="51">MIN(MAX(F$151-(G66-G65),0),F77)</f>
         <v>0</v>
       </c>
       <c r="G79" s="274">
-        <f t="shared" ref="G79:O79" si="49">MIN(MAX(G$151-(I66-I65),0),G77)</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="H79" s="274">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="I79" s="274">
-        <f t="shared" si="49"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="J79" s="274">
-        <f t="shared" si="49"/>
-        <v>0</v>
+        <f>MIN(MAX(J$151-(K66-K65),0),J77)</f>
+        <v>15</v>
       </c>
       <c r="K79" s="274">
-        <f t="shared" si="49"/>
+        <f t="shared" ref="K79:O79" si="52">MIN(MAX(K$151-(L66-L65),0),K77)</f>
         <v>0</v>
       </c>
       <c r="L79" s="274">
-        <f t="shared" si="49"/>
-        <v>0</v>
+        <f t="shared" si="52"/>
+        <v>10</v>
       </c>
       <c r="M79" s="274">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N79" s="274">
-        <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="O79" s="274" t="e">
-        <f t="shared" si="49"/>
-        <v>#VALUE!</v>
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="O79" s="274">
+        <f t="shared" si="52"/>
+        <v>0</v>
       </c>
       <c r="P79" s="50"/>
       <c r="AC79" s="117"/>
@@ -10186,39 +10182,39 @@
         <v>0</v>
       </c>
       <c r="G80" s="85">
-        <f t="shared" ref="G80:O80" si="50">QUOTIENT(MOD(G78+$E$50-1,$E$49),$E$50)</f>
+        <f t="shared" ref="G80:O80" si="53">QUOTIENT(MOD(G78+$E$50-1,$E$49),$E$50)</f>
         <v>0</v>
       </c>
       <c r="H80" s="85">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="I80" s="85">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="J80" s="85">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="K80" s="85">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="L80" s="85">
-        <f t="shared" si="50"/>
-        <v>0</v>
+        <f t="shared" si="53"/>
+        <v>1</v>
       </c>
       <c r="M80" s="85">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="N80" s="85">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="O80" s="86">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="P80" s="58"/>
@@ -10276,39 +10272,39 @@
         <v>0</v>
       </c>
       <c r="G81" s="85">
-        <f t="shared" ref="G81:O81" si="51">QUOTIENT(G78+$E$50-1,$E$49)</f>
+        <f t="shared" ref="G81:O81" si="54">QUOTIENT(G78+$E$50-1,$E$49)</f>
         <v>0</v>
       </c>
       <c r="H81" s="85">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="I81" s="85">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="J81" s="85">
-        <f t="shared" si="51"/>
-        <v>0</v>
+        <f t="shared" si="54"/>
+        <v>1</v>
       </c>
       <c r="K81" s="85">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="L81" s="85">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="M81" s="85">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="N81" s="85">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="O81" s="86">
-        <f t="shared" si="51"/>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="P81" s="58"/>
@@ -10366,39 +10362,39 @@
         <v>0</v>
       </c>
       <c r="G82" s="132">
-        <f t="shared" ref="G82:O82" si="52">G81*$F$49+G80*$F$50</f>
+        <f t="shared" ref="G82:O82" si="55">G81*$F$49+G80*$F$50</f>
         <v>0</v>
       </c>
       <c r="H82" s="132">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="I82" s="132">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="J82" s="132">
-        <f t="shared" si="52"/>
-        <v>0</v>
+        <f t="shared" si="55"/>
+        <v>500</v>
       </c>
       <c r="K82" s="132">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="L82" s="132">
-        <f t="shared" si="52"/>
-        <v>0</v>
+        <f t="shared" si="55"/>
+        <v>280</v>
       </c>
       <c r="M82" s="132">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="N82" s="132">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="O82" s="133">
-        <f t="shared" si="52"/>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="P82" s="134"/>
@@ -10455,43 +10451,43 @@
       </c>
       <c r="E83" s="92"/>
       <c r="F83" s="140">
-        <f>F78*F71</f>
+        <f t="shared" ref="F83:I83" si="56">F79*F71</f>
         <v>0</v>
       </c>
       <c r="G83" s="140">
-        <f t="shared" ref="G83:O83" si="53">G78*G71</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="H83" s="140">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I83" s="140">
-        <f t="shared" si="53"/>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="J83" s="140">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f>J79*J71</f>
+        <v>3225</v>
       </c>
       <c r="K83" s="140">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="K83:O83" si="57">K79*K71</f>
         <v>0</v>
       </c>
       <c r="L83" s="140">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f t="shared" si="57"/>
+        <v>2140</v>
       </c>
       <c r="M83" s="140">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="N83" s="140">
-        <f t="shared" si="53"/>
-        <v>0</v>
-      </c>
-      <c r="O83" s="141">
-        <f t="shared" si="53"/>
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="O83" s="140">
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="P83" s="134"/>
@@ -10550,39 +10546,39 @@
         <v>0</v>
       </c>
       <c r="G84" s="110">
-        <f t="shared" ref="G84:O84" si="54">G83+G82</f>
+        <f t="shared" ref="G84:O84" si="58">G83+G82</f>
         <v>0</v>
       </c>
       <c r="H84" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="I84" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="J84" s="110">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" si="58"/>
+        <v>3725</v>
       </c>
       <c r="K84" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="L84" s="110">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f t="shared" si="58"/>
+        <v>2420</v>
       </c>
       <c r="M84" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="N84" s="110">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="O84" s="111">
-        <f t="shared" si="54"/>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="P84" s="58"/>
@@ -10594,43 +10590,43 @@
       </c>
       <c r="E85" s="92"/>
       <c r="F85" s="140">
-        <f>F78*F74</f>
+        <f t="shared" ref="F85:I85" si="59">F79*F74</f>
         <v>0</v>
       </c>
       <c r="G85" s="140">
-        <f t="shared" ref="G85:O85" si="55">G78*G74</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="H85" s="140">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="I85" s="140">
-        <f t="shared" si="55"/>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="J85" s="140">
-        <f t="shared" si="55"/>
-        <v>0</v>
+        <f>J79*J74</f>
+        <v>6270</v>
       </c>
       <c r="K85" s="140">
-        <f t="shared" si="55"/>
+        <f t="shared" ref="K85:O85" si="60">K79*K74</f>
         <v>0</v>
       </c>
       <c r="L85" s="140">
-        <f t="shared" si="55"/>
-        <v>0</v>
+        <f t="shared" si="60"/>
+        <v>4260</v>
       </c>
       <c r="M85" s="140">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="N85" s="140">
-        <f t="shared" si="55"/>
-        <v>0</v>
-      </c>
-      <c r="O85" s="141">
-        <f t="shared" si="55"/>
+        <f t="shared" si="60"/>
+        <v>0</v>
+      </c>
+      <c r="O85" s="140">
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="P85" s="58"/>
@@ -10650,35 +10646,35 @@
         <v>0</v>
       </c>
       <c r="H86" s="144">
-        <f t="shared" ref="H86:O86" si="56">H85-H84</f>
+        <f t="shared" ref="H86:O86" si="61">H85-H84</f>
         <v>0</v>
       </c>
       <c r="I86" s="143">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="J86" s="143">
-        <f t="shared" si="56"/>
-        <v>0</v>
+        <f t="shared" si="61"/>
+        <v>2545</v>
       </c>
       <c r="K86" s="143">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="L86" s="143">
-        <f t="shared" si="56"/>
-        <v>0</v>
+        <f t="shared" si="61"/>
+        <v>1840</v>
       </c>
       <c r="M86" s="143">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="N86" s="143">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="O86" s="145">
-        <f t="shared" si="56"/>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="P86" s="50" t="s">
@@ -10700,35 +10696,35 @@
         <v>0</v>
       </c>
       <c r="H87" s="148">
-        <f t="shared" ref="H87:O87" si="57">H76-H86</f>
+        <f t="shared" ref="H87:O87" si="62">H76-H86</f>
         <v>13920</v>
       </c>
       <c r="I87" s="148">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>17300</v>
       </c>
       <c r="J87" s="148">
-        <f t="shared" si="57"/>
-        <v>3560</v>
+        <f t="shared" si="62"/>
+        <v>1015</v>
       </c>
       <c r="K87" s="148">
-        <f t="shared" si="57"/>
-        <v>33660</v>
+        <f t="shared" si="62"/>
+        <v>37400</v>
       </c>
       <c r="L87" s="148">
-        <f t="shared" si="57"/>
-        <v>3740</v>
+        <f t="shared" si="62"/>
+        <v>-1840</v>
       </c>
       <c r="M87" s="148">
-        <f t="shared" si="57"/>
-        <v>7280</v>
+        <f t="shared" si="62"/>
+        <v>10920</v>
       </c>
       <c r="N87" s="148">
-        <f t="shared" si="57"/>
-        <v>3600</v>
+        <f t="shared" si="62"/>
+        <v>0</v>
       </c>
       <c r="O87" s="149">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="AA87" s="169"/>
@@ -10739,43 +10735,43 @@
       </c>
       <c r="E88" s="151"/>
       <c r="F88" s="152">
-        <f t="shared" ref="F88:O88" si="58">F77/F67</f>
+        <f t="shared" ref="F88:O88" si="63">F77/F67</f>
         <v>0.5</v>
       </c>
       <c r="G88" s="152" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H88" s="152">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>0.25</v>
       </c>
       <c r="I88" s="152">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>0.2</v>
       </c>
       <c r="J88" s="152">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>0.75</v>
       </c>
       <c r="K88" s="152">
-        <f t="shared" si="58"/>
-        <v>0.80555555555555558</v>
-      </c>
-      <c r="L88" s="152">
-        <f t="shared" si="58"/>
-        <v>0.5</v>
+        <f t="shared" si="63"/>
+        <v>0.75</v>
+      </c>
+      <c r="L88" s="152" t="e">
+        <f t="shared" si="63"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="M88" s="152">
-        <f t="shared" si="58"/>
-        <v>0</v>
-      </c>
-      <c r="N88" s="152">
-        <f t="shared" si="58"/>
-        <v>0.5</v>
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="N88" s="152" t="e">
+        <f t="shared" si="63"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="O88" s="152" t="e">
-        <f t="shared" si="58"/>
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA88" s="169"/>
@@ -10786,43 +10782,43 @@
       </c>
       <c r="E89" s="151"/>
       <c r="F89" s="152">
-        <f t="shared" ref="F89:O89" si="59">F84/F73</f>
+        <f t="shared" ref="F89:O89" si="64">F84/F73</f>
         <v>0</v>
       </c>
       <c r="G89" s="152" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H89" s="152">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I89" s="152">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="J89" s="152">
-        <f t="shared" si="59"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>0.77604166666666663</v>
       </c>
       <c r="K89" s="152">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="L89" s="152">
-        <f t="shared" si="59"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="L89" s="152" t="e">
+        <f t="shared" si="64"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="M89" s="152">
-        <f t="shared" si="59"/>
-        <v>0</v>
-      </c>
-      <c r="N89" s="152">
-        <f t="shared" si="59"/>
-        <v>0</v>
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="N89" s="152" t="e">
+        <f t="shared" si="64"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="O89" s="152" t="e">
-        <f t="shared" si="59"/>
+        <f t="shared" si="64"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA89" s="169"/>
@@ -10833,43 +10829,43 @@
       </c>
       <c r="E90" s="153"/>
       <c r="F90" s="152">
-        <f t="shared" ref="F90:O90" si="60">F86/F76</f>
+        <f t="shared" ref="F90:O90" si="65">F86/F76</f>
         <v>0</v>
       </c>
       <c r="G90" s="152" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H90" s="152">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="I90" s="152">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="J90" s="152">
-        <f t="shared" si="60"/>
-        <v>0</v>
+        <f t="shared" si="65"/>
+        <v>0.7148876404494382</v>
       </c>
       <c r="K90" s="152">
-        <f t="shared" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="L90" s="152">
-        <f t="shared" si="60"/>
-        <v>0</v>
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="L90" s="152" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="M90" s="152">
-        <f t="shared" si="60"/>
-        <v>0</v>
-      </c>
-      <c r="N90" s="152">
-        <f t="shared" si="60"/>
-        <v>0</v>
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+      <c r="N90" s="152" t="e">
+        <f t="shared" si="65"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="O90" s="152" t="e">
-        <f t="shared" si="60"/>
+        <f t="shared" si="65"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AA90" s="169"/>
@@ -11087,7 +11083,7 @@
       </c>
       <c r="L103" s="67">
         <f>'DC3'!I13</f>
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="M103" s="67">
         <f>'DC3'!J13</f>
@@ -11250,39 +11246,39 @@
         <v>10</v>
       </c>
       <c r="G107" s="214">
-        <f t="shared" ref="G107:O107" si="61">SUM(G103:G106)</f>
+        <f t="shared" ref="G107:O107" si="66">SUM(G103:G106)</f>
         <v>20</v>
       </c>
       <c r="H107" s="214">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>40</v>
       </c>
       <c r="I107" s="214">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>50</v>
       </c>
       <c r="J107" s="214">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>50</v>
       </c>
       <c r="K107" s="214">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>20</v>
       </c>
       <c r="L107" s="214">
-        <f t="shared" si="61"/>
-        <v>140</v>
+        <f t="shared" si="66"/>
+        <v>180</v>
       </c>
       <c r="M107" s="214">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>15</v>
       </c>
       <c r="N107" s="214">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>30</v>
       </c>
       <c r="O107" s="215">
-        <f t="shared" si="61"/>
+        <f t="shared" si="66"/>
         <v>20</v>
       </c>
     </row>
@@ -11321,39 +11317,39 @@
         <v>30</v>
       </c>
       <c r="G109" s="177">
-        <f t="shared" ref="G109:O109" si="62">F109+G108+G111-G107</f>
+        <f t="shared" ref="G109:O109" si="67">F109+G108+G111-G107</f>
         <v>10</v>
       </c>
       <c r="H109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>10</v>
       </c>
       <c r="I109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>10</v>
       </c>
       <c r="J109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>10</v>
       </c>
       <c r="K109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>10</v>
       </c>
       <c r="L109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>10</v>
       </c>
       <c r="M109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="N109" s="177">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="O109" s="178">
-        <f t="shared" si="62"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="Q109" s="72" t="s">
@@ -11370,39 +11366,39 @@
         <v>0</v>
       </c>
       <c r="G110" s="177">
-        <f t="shared" ref="G110:O110" si="63">IF(F109-G107&lt;=$E$101, G107-F109+$E$101,0)</f>
+        <f t="shared" ref="G110:O110" si="68">IF(F109-G107&lt;=$E$101, G107-F109+$E$101,0)</f>
         <v>0</v>
       </c>
       <c r="H110" s="177">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>40</v>
       </c>
       <c r="I110" s="177">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>50</v>
       </c>
       <c r="J110" s="177">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>50</v>
       </c>
       <c r="K110" s="177">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>20</v>
       </c>
       <c r="L110" s="177">
-        <f t="shared" si="63"/>
-        <v>140</v>
+        <f t="shared" si="68"/>
+        <v>180</v>
       </c>
       <c r="M110" s="177">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>15</v>
       </c>
       <c r="N110" s="177">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>25</v>
       </c>
       <c r="O110" s="178">
-        <f t="shared" si="63"/>
+        <f t="shared" si="68"/>
         <v>15</v>
       </c>
       <c r="Q110" s="72" t="s">
@@ -11419,39 +11415,39 @@
         <v>0</v>
       </c>
       <c r="G111" s="177">
-        <f t="shared" ref="G111:O111" si="64" xml:space="preserve"> CEILING(G110/$E$100,1)*$E$100</f>
+        <f t="shared" ref="G111:O111" si="69" xml:space="preserve"> CEILING(G110/$E$100,1)*$E$100</f>
         <v>0</v>
       </c>
       <c r="H111" s="177">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>40</v>
       </c>
       <c r="I111" s="177">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>50</v>
       </c>
       <c r="J111" s="177">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>50</v>
       </c>
       <c r="K111" s="177">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>20</v>
       </c>
       <c r="L111" s="177">
-        <f t="shared" si="64"/>
-        <v>140</v>
+        <f t="shared" si="69"/>
+        <v>180</v>
       </c>
       <c r="M111" s="177">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>20</v>
       </c>
       <c r="N111" s="177">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>30</v>
       </c>
       <c r="O111" s="178">
-        <f t="shared" si="64"/>
+        <f t="shared" si="69"/>
         <v>20</v>
       </c>
     </row>
@@ -11461,43 +11457,43 @@
       </c>
       <c r="E112" s="182"/>
       <c r="F112" s="183">
-        <f t="shared" ref="F112:O112" si="65">F111</f>
+        <f t="shared" ref="F112:O112" si="70">F111</f>
         <v>0</v>
       </c>
       <c r="G112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="H112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>40</v>
       </c>
       <c r="I112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>50</v>
       </c>
       <c r="J112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>50</v>
       </c>
       <c r="K112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>20</v>
       </c>
       <c r="L112" s="183">
-        <f t="shared" si="65"/>
-        <v>140</v>
+        <f t="shared" si="70"/>
+        <v>180</v>
       </c>
       <c r="M112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>20</v>
       </c>
       <c r="N112" s="183">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>30</v>
       </c>
       <c r="O112" s="184">
-        <f t="shared" si="65"/>
+        <f t="shared" si="70"/>
         <v>20</v>
       </c>
     </row>
@@ -11511,7 +11507,7 @@
         <v>0</v>
       </c>
       <c r="G113" s="81">
-        <f t="shared" ref="G113:O113" si="66">QUOTIENT(MOD(G112+$E$95-1,$E$94),$E$95)</f>
+        <f t="shared" ref="G113:O113" si="71">QUOTIENT(MOD(G112+$E$95-1,$E$94),$E$95)</f>
         <v>0</v>
       </c>
       <c r="H113" s="81">
@@ -11519,31 +11515,31 @@
         <v>0</v>
       </c>
       <c r="I113" s="81">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="J113" s="81">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="K113" s="81">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="L113" s="81">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="M113" s="81">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="N113" s="81">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="O113" s="82">
-        <f t="shared" si="66"/>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
     </row>
@@ -11558,39 +11554,39 @@
         <v>0</v>
       </c>
       <c r="G114" s="85">
-        <f t="shared" ref="G114:O114" si="67">QUOTIENT(G112+$E$95-1,$E$94)</f>
+        <f t="shared" ref="G114:O114" si="72">QUOTIENT(G112+$E$95-1,$E$94)</f>
         <v>0</v>
       </c>
       <c r="H114" s="85">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>2</v>
       </c>
       <c r="I114" s="85">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>2</v>
       </c>
       <c r="J114" s="85">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>2</v>
       </c>
       <c r="K114" s="85">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="L114" s="85">
-        <f t="shared" si="67"/>
-        <v>7</v>
+        <f t="shared" si="72"/>
+        <v>9</v>
       </c>
       <c r="M114" s="85">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="N114" s="85">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="O114" s="86">
-        <f t="shared" si="67"/>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
     </row>
@@ -11604,39 +11600,39 @@
         <v>0</v>
       </c>
       <c r="G115" s="89">
-        <f t="shared" ref="G115:O115" si="68">G114*$F$94+G113*$F$95</f>
+        <f t="shared" ref="G115:O115" si="73">G114*$F$94+G113*$F$95</f>
         <v>0</v>
       </c>
       <c r="H115" s="89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>400</v>
       </c>
       <c r="I115" s="89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>520</v>
       </c>
       <c r="J115" s="89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>520</v>
       </c>
       <c r="K115" s="89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>200</v>
       </c>
       <c r="L115" s="89">
-        <f t="shared" si="68"/>
-        <v>1400</v>
+        <f t="shared" si="73"/>
+        <v>1800</v>
       </c>
       <c r="M115" s="89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>200</v>
       </c>
       <c r="N115" s="89">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>320</v>
       </c>
       <c r="O115" s="90">
-        <f t="shared" si="68"/>
+        <f t="shared" si="73"/>
         <v>200</v>
       </c>
     </row>
@@ -11699,39 +11695,39 @@
         <v>0</v>
       </c>
       <c r="G117" s="97">
-        <f t="shared" ref="G117:O117" si="69">G116*G112</f>
+        <f t="shared" ref="G117:O117" si="74">G116*G112</f>
         <v>0</v>
       </c>
       <c r="H117" s="97">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>8520</v>
       </c>
       <c r="I117" s="97">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>10750</v>
       </c>
       <c r="J117" s="97">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>10750</v>
       </c>
       <c r="K117" s="97">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>4320</v>
       </c>
       <c r="L117" s="97">
-        <f t="shared" si="69"/>
-        <v>29960</v>
+        <f t="shared" si="74"/>
+        <v>38520</v>
       </c>
       <c r="M117" s="97">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>4240</v>
       </c>
       <c r="N117" s="97">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>6300</v>
       </c>
       <c r="O117" s="136">
-        <f t="shared" si="69"/>
+        <f t="shared" si="74"/>
         <v>4180</v>
       </c>
       <c r="P117" s="50" t="s">
@@ -11744,43 +11740,43 @@
       </c>
       <c r="E118" s="101"/>
       <c r="F118" s="102">
-        <f t="shared" ref="F118:O118" si="70">F115+F117</f>
+        <f t="shared" ref="F118:O118" si="75">F115+F117</f>
         <v>0</v>
       </c>
       <c r="G118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="H118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>8920</v>
       </c>
       <c r="I118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>11270</v>
       </c>
       <c r="J118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>11270</v>
       </c>
       <c r="K118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>4520</v>
       </c>
       <c r="L118" s="102">
-        <f t="shared" si="70"/>
-        <v>31360</v>
+        <f t="shared" si="75"/>
+        <v>40320</v>
       </c>
       <c r="M118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>4440</v>
       </c>
       <c r="N118" s="102">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>6620</v>
       </c>
       <c r="O118" s="103">
-        <f t="shared" si="70"/>
+        <f t="shared" si="75"/>
         <v>4380</v>
       </c>
       <c r="P118" s="50" t="s">
@@ -11843,39 +11839,39 @@
         <v>0</v>
       </c>
       <c r="G120" s="106">
-        <f t="shared" ref="G120:O120" si="71">G119*G112</f>
+        <f t="shared" ref="G120:O120" si="76">G119*G112</f>
         <v>0</v>
       </c>
       <c r="H120" s="106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>16400</v>
       </c>
       <c r="I120" s="106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>20750</v>
       </c>
       <c r="J120" s="106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>20900</v>
       </c>
       <c r="K120" s="106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>8600</v>
       </c>
       <c r="L120" s="106">
-        <f t="shared" si="71"/>
-        <v>59220</v>
+        <f t="shared" si="76"/>
+        <v>76140</v>
       </c>
       <c r="M120" s="106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>8380</v>
       </c>
       <c r="N120" s="106">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>12510</v>
       </c>
       <c r="O120" s="107">
-        <f t="shared" si="71"/>
+        <f t="shared" si="76"/>
         <v>8440</v>
       </c>
       <c r="P120" s="50" t="s">
@@ -11892,39 +11888,39 @@
         <v>0</v>
       </c>
       <c r="G121" s="110">
-        <f t="shared" ref="G121:O121" si="72">G120-G118</f>
+        <f t="shared" ref="G121:O121" si="77">G120-G118</f>
         <v>0</v>
       </c>
       <c r="H121" s="110">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>7480</v>
       </c>
       <c r="I121" s="110">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>9480</v>
       </c>
       <c r="J121" s="110">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>9630</v>
       </c>
       <c r="K121" s="110">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>4080</v>
       </c>
       <c r="L121" s="110">
-        <f t="shared" si="72"/>
-        <v>27860</v>
+        <f t="shared" si="77"/>
+        <v>35820</v>
       </c>
       <c r="M121" s="110">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>3940</v>
       </c>
       <c r="N121" s="110">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>5890</v>
       </c>
       <c r="O121" s="111">
-        <f t="shared" si="72"/>
+        <f t="shared" si="77"/>
         <v>4060</v>
       </c>
       <c r="P121" s="50" t="s">
@@ -11941,39 +11937,39 @@
         <v>10</v>
       </c>
       <c r="G122" s="223">
-        <f t="shared" ref="G122:O122" si="73">SUM(G103:G104)</f>
+        <f t="shared" ref="G122:O122" si="78">SUM(G103:G104)</f>
         <v>0</v>
       </c>
       <c r="H122" s="223">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="I122" s="223">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>20</v>
       </c>
       <c r="J122" s="223">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>10</v>
       </c>
       <c r="K122" s="223">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="L122" s="223">
-        <f t="shared" si="73"/>
-        <v>110</v>
+        <f t="shared" si="78"/>
+        <v>150</v>
       </c>
       <c r="M122" s="223">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>15</v>
       </c>
       <c r="N122" s="223">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="O122" s="224">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="P122" s="50" t="s">
@@ -11986,43 +11982,43 @@
       </c>
       <c r="E123" s="112"/>
       <c r="F123" s="81">
-        <f t="shared" ref="F123:O123" si="74">MIN(F151,F122)</f>
+        <f t="shared" ref="F123:O123" si="79">MIN(F151,F122)</f>
         <v>0</v>
       </c>
       <c r="G123" s="81">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="H123" s="81">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="I123" s="81">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="J123" s="81">
-        <f t="shared" si="74"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>10</v>
       </c>
       <c r="K123" s="81">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="L123" s="81">
-        <f t="shared" si="74"/>
-        <v>0</v>
+        <f t="shared" si="79"/>
+        <v>20</v>
       </c>
       <c r="M123" s="81">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="N123" s="81">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="O123" s="82">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="P123" s="50" t="s">
@@ -12032,15 +12028,15 @@
         <v>38</v>
       </c>
       <c r="X123">
-        <f t="shared" ref="X123" si="75">CEILING(W123,20)</f>
+        <f t="shared" ref="X123" si="80">CEILING(W123,20)</f>
         <v>40</v>
       </c>
       <c r="Y123">
-        <f t="shared" ref="Y123" si="76">FLOOR(W123,20)</f>
+        <f t="shared" ref="Y123" si="81">FLOOR(W123,20)</f>
         <v>20</v>
       </c>
       <c r="Z123">
-        <f t="shared" ref="Z123" si="77">MOD(W123,20)</f>
+        <f t="shared" ref="Z123" si="82">MOD(W123,20)</f>
         <v>18</v>
       </c>
       <c r="AA123" s="120">
@@ -12056,19 +12052,19 @@
         <v>2</v>
       </c>
       <c r="AE123">
-        <f t="shared" ref="AE123" si="78">QUOTIENT(MOD(W123,$AD$29),$AD$28)</f>
+        <f t="shared" ref="AE123" si="83">QUOTIENT(MOD(W123,$AD$29),$AD$28)</f>
         <v>1</v>
       </c>
       <c r="AF123" s="128">
-        <f t="shared" ref="AF123" si="79">QUOTIENT(MOD(W123+$AD$28-1,$AD$29),$AD$28)</f>
+        <f t="shared" ref="AF123" si="84">QUOTIENT(MOD(W123+$AD$28-1,$AD$29),$AD$28)</f>
         <v>0</v>
       </c>
       <c r="AG123">
-        <f t="shared" ref="AG123" si="80">QUOTIENT(W123,$AD$29)</f>
+        <f t="shared" ref="AG123" si="85">QUOTIENT(W123,$AD$29)</f>
         <v>1</v>
       </c>
       <c r="AH123" s="129">
-        <f t="shared" ref="AH123" si="81">QUOTIENT(W123+$AD$28-1,$AD$29)</f>
+        <f t="shared" ref="AH123" si="86">QUOTIENT(W123+$AD$28-1,$AD$29)</f>
         <v>2</v>
       </c>
     </row>
@@ -12078,42 +12074,43 @@
       </c>
       <c r="E124" s="273"/>
       <c r="F124" s="274">
-        <f>MIN(MAX(F$151-(H111-H110),0),F122)</f>
+        <f t="shared" ref="F124:I124" si="87">MIN(MAX(F$151-(F111-F110),0),F122)</f>
         <v>0</v>
       </c>
       <c r="G124" s="274">
-        <f t="shared" ref="G124:N124" si="82">MIN(MAX(G$151-(I111-I110),0),G122)</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="H124" s="274">
-        <f t="shared" si="82"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="I124" s="274">
-        <f t="shared" si="82"/>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="J124" s="274">
-        <f t="shared" si="82"/>
-        <v>0</v>
+        <f>MIN(MAX(J$151-(J111-J110),0),J122)</f>
+        <v>10</v>
       </c>
       <c r="K124" s="274">
-        <f t="shared" si="82"/>
+        <f t="shared" ref="K124:O124" si="88">MIN(MAX(K$151-(K111-K110),0),K122)</f>
         <v>0</v>
       </c>
       <c r="L124" s="274">
-        <f t="shared" si="82"/>
-        <v>0</v>
+        <f t="shared" si="88"/>
+        <v>20</v>
       </c>
       <c r="M124" s="274">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="N124" s="274">
-        <f t="shared" si="82"/>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="O124" s="275">
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="P124" s="50"/>
@@ -12130,43 +12127,43 @@
       </c>
       <c r="E125" s="161"/>
       <c r="F125" s="85">
-        <f t="shared" ref="F125:O125" si="83">QUOTIENT(MOD(F123+$E$95-1,$E$94),$E$95)</f>
+        <f t="shared" ref="F125:O125" si="89">QUOTIENT(MOD(F123+$E$95-1,$E$94),$E$95)</f>
         <v>0</v>
       </c>
       <c r="G125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="H125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="I125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="J125" s="85">
-        <f t="shared" si="83"/>
-        <v>0</v>
+        <f t="shared" si="89"/>
+        <v>1</v>
       </c>
       <c r="K125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="L125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="M125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="N125" s="85">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="O125" s="86">
-        <f t="shared" si="83"/>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="P125" s="58"/>
@@ -12177,43 +12174,43 @@
       </c>
       <c r="E126" s="84"/>
       <c r="F126" s="85">
-        <f t="shared" ref="F126:O126" si="84">QUOTIENT(F123+$E$95-1,$E$94)</f>
+        <f t="shared" ref="F126:O126" si="90">QUOTIENT(F123+$E$95-1,$E$94)</f>
         <v>0</v>
       </c>
       <c r="G126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="I126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="J126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="K126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="L126" s="85">
-        <f t="shared" si="84"/>
-        <v>0</v>
+        <f t="shared" si="90"/>
+        <v>1</v>
       </c>
       <c r="M126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="N126" s="85">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="O126" s="86">
-        <f t="shared" si="84"/>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="P126" s="58"/>
@@ -12228,39 +12225,39 @@
         <v>0</v>
       </c>
       <c r="G127" s="132">
-        <f t="shared" ref="G127:O127" si="85">G126*$F$94+G125*$F$95</f>
+        <f t="shared" ref="G127:O127" si="91">G126*$F$94+G125*$F$95</f>
         <v>0</v>
       </c>
       <c r="H127" s="132">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="I127" s="132">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="J127" s="132">
-        <f t="shared" si="85"/>
-        <v>0</v>
+        <f t="shared" si="91"/>
+        <v>120</v>
       </c>
       <c r="K127" s="132">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="L127" s="132">
-        <f t="shared" si="85"/>
-        <v>0</v>
+        <f t="shared" si="91"/>
+        <v>200</v>
       </c>
       <c r="M127" s="132">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="N127" s="132">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="O127" s="133">
-        <f t="shared" si="85"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="P127" s="134"/>
@@ -12274,43 +12271,43 @@
       </c>
       <c r="E128" s="92"/>
       <c r="F128" s="140">
-        <f t="shared" ref="F128:O128" si="86">F123*F116</f>
+        <f t="shared" ref="F128:I128" si="92">F124*F116</f>
         <v>0</v>
       </c>
       <c r="G128" s="140">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="H128" s="140">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="I128" s="140">
-        <f t="shared" si="86"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="J128" s="140">
-        <f t="shared" si="86"/>
-        <v>0</v>
+        <f>J124*J116</f>
+        <v>2150</v>
       </c>
       <c r="K128" s="140">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="K128:O128" si="93">K124*K116</f>
         <v>0</v>
       </c>
       <c r="L128" s="140">
-        <f t="shared" si="86"/>
-        <v>0</v>
+        <f t="shared" si="93"/>
+        <v>4280</v>
       </c>
       <c r="M128" s="140">
-        <f t="shared" si="86"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="N128" s="140">
-        <f t="shared" si="86"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="O128" s="141">
-        <f t="shared" si="86"/>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="P128" s="134"/>
@@ -12326,39 +12323,39 @@
         <v>0</v>
       </c>
       <c r="G129" s="110">
-        <f t="shared" ref="G129:O129" si="87">G128+G127</f>
+        <f t="shared" ref="G129:O129" si="94">G128+G127</f>
         <v>0</v>
       </c>
       <c r="H129" s="110">
-        <f t="shared" si="87"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="I129" s="110">
-        <f t="shared" si="87"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="J129" s="110">
-        <f t="shared" si="87"/>
-        <v>0</v>
+        <f t="shared" si="94"/>
+        <v>2270</v>
       </c>
       <c r="K129" s="110">
-        <f t="shared" si="87"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="L129" s="110">
-        <f t="shared" si="87"/>
-        <v>0</v>
+        <f t="shared" si="94"/>
+        <v>4480</v>
       </c>
       <c r="M129" s="110">
-        <f t="shared" si="87"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="N129" s="110">
-        <f t="shared" si="87"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="O129" s="111">
-        <f t="shared" si="87"/>
+        <f t="shared" si="94"/>
         <v>0</v>
       </c>
       <c r="P129" s="58"/>
@@ -12369,43 +12366,43 @@
       </c>
       <c r="E130" s="92"/>
       <c r="F130" s="140">
-        <f t="shared" ref="F130:O130" si="88">F123*F119</f>
+        <f t="shared" ref="F130:I130" si="95">F124*F119</f>
         <v>0</v>
       </c>
       <c r="G130" s="140">
-        <f t="shared" si="88"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="H130" s="140">
-        <f t="shared" si="88"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="I130" s="140">
-        <f t="shared" si="88"/>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="J130" s="140">
-        <f t="shared" si="88"/>
-        <v>0</v>
+        <f>J124*J119</f>
+        <v>4180</v>
       </c>
       <c r="K130" s="140">
-        <f t="shared" si="88"/>
+        <f t="shared" ref="K130:O130" si="96">K124*K119</f>
         <v>0</v>
       </c>
       <c r="L130" s="140">
-        <f t="shared" si="88"/>
-        <v>0</v>
+        <f t="shared" si="96"/>
+        <v>8460</v>
       </c>
       <c r="M130" s="140">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="N130" s="140">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="O130" s="141">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="P130" s="58"/>
@@ -12424,35 +12421,35 @@
         <v>0</v>
       </c>
       <c r="H131" s="144">
-        <f t="shared" ref="H131:O131" si="89">H130-H129</f>
+        <f t="shared" ref="H131:O131" si="97">H130-H129</f>
         <v>0</v>
       </c>
       <c r="I131" s="143">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="J131" s="143">
-        <f t="shared" si="89"/>
-        <v>0</v>
+        <f t="shared" si="97"/>
+        <v>1910</v>
       </c>
       <c r="K131" s="143">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="L131" s="143">
-        <f t="shared" si="89"/>
-        <v>0</v>
+        <f t="shared" si="97"/>
+        <v>3980</v>
       </c>
       <c r="M131" s="143">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="N131" s="143">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="O131" s="145">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="P131" s="50" t="s">
@@ -12465,43 +12462,43 @@
       </c>
       <c r="E132" s="147"/>
       <c r="F132" s="148">
-        <f t="shared" ref="F132:O132" si="90">F121-F131</f>
+        <f t="shared" ref="F132:O132" si="98">F121-F131</f>
         <v>0</v>
       </c>
       <c r="G132" s="148">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>0</v>
       </c>
       <c r="H132" s="148">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>7480</v>
       </c>
       <c r="I132" s="148">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>9480</v>
       </c>
       <c r="J132" s="148">
-        <f t="shared" si="90"/>
-        <v>9630</v>
+        <f t="shared" si="98"/>
+        <v>7720</v>
       </c>
       <c r="K132" s="148">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>4080</v>
       </c>
       <c r="L132" s="148">
-        <f t="shared" si="90"/>
-        <v>27860</v>
+        <f t="shared" si="98"/>
+        <v>31840</v>
       </c>
       <c r="M132" s="148">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>3940</v>
       </c>
       <c r="N132" s="148">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>5890</v>
       </c>
       <c r="O132" s="149">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>4060</v>
       </c>
       <c r="AA132" s="169"/>
@@ -12512,43 +12509,43 @@
       </c>
       <c r="E133" s="151"/>
       <c r="F133" s="152" t="e">
-        <f t="shared" ref="F133:O133" si="91">F122/F112</f>
+        <f t="shared" ref="F133:O133" si="99">F122/F112</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G133" s="152" t="e">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="I133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0.4</v>
       </c>
       <c r="J133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0.2</v>
       </c>
       <c r="K133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="L133" s="152">
-        <f t="shared" si="91"/>
-        <v>0.7857142857142857</v>
+        <f t="shared" si="99"/>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0.75</v>
       </c>
       <c r="N133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="O133" s="152">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0</v>
       </c>
       <c r="AA133" s="169"/>
@@ -12559,43 +12556,43 @@
       </c>
       <c r="E134" s="151"/>
       <c r="F134" s="152" t="e">
-        <f t="shared" ref="F134:O134" si="92">F129/F118</f>
+        <f t="shared" ref="F134:O134" si="100">F129/F118</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G134" s="152" t="e">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H134" s="152">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="I134" s="152">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="J134" s="152">
-        <f t="shared" si="92"/>
-        <v>0</v>
+        <f t="shared" si="100"/>
+        <v>0.20141969831410825</v>
       </c>
       <c r="K134" s="152">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="L134" s="152">
-        <f t="shared" si="92"/>
-        <v>0</v>
+        <f t="shared" si="100"/>
+        <v>0.1111111111111111</v>
       </c>
       <c r="M134" s="152">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="N134" s="152">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="O134" s="152">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="AA134" s="169"/>
@@ -12606,43 +12603,43 @@
       </c>
       <c r="E135" s="153"/>
       <c r="F135" s="152" t="e">
-        <f t="shared" ref="F135:O135" si="93">F131/F121</f>
+        <f t="shared" ref="F135:O135" si="101">F131/F121</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G135" s="152" t="e">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H135" s="152">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="I135" s="152">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="J135" s="152">
-        <f t="shared" si="93"/>
-        <v>0</v>
+        <f t="shared" si="101"/>
+        <v>0.19833852544132918</v>
       </c>
       <c r="K135" s="152">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="L135" s="152">
-        <f t="shared" si="93"/>
-        <v>0</v>
+        <f t="shared" si="101"/>
+        <v>0.1111111111111111</v>
       </c>
       <c r="M135" s="152">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="N135" s="152">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
       <c r="O135" s="152">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>0</v>
       </c>
     </row>
@@ -12774,43 +12771,43 @@
       </c>
       <c r="E145" s="192"/>
       <c r="F145" s="193">
-        <f t="shared" ref="F145:O145" si="94">SUM(F112,F67,F23)</f>
+        <f t="shared" ref="F145:O145" si="102">SUM(F112,F67,F23)</f>
         <v>20</v>
       </c>
       <c r="G145" s="193">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>80</v>
       </c>
       <c r="H145" s="193">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>220</v>
       </c>
       <c r="I145" s="193">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>170</v>
       </c>
       <c r="J145" s="193">
-        <f t="shared" si="94"/>
-        <v>230</v>
+        <f t="shared" si="102"/>
+        <v>260</v>
       </c>
       <c r="K145" s="193">
-        <f t="shared" si="94"/>
-        <v>200</v>
+        <f t="shared" si="102"/>
+        <v>220</v>
       </c>
       <c r="L145" s="193">
-        <f t="shared" si="94"/>
-        <v>200</v>
+        <f t="shared" si="102"/>
+        <v>220</v>
       </c>
       <c r="M145" s="193">
-        <f t="shared" si="94"/>
-        <v>70</v>
+        <f t="shared" si="102"/>
+        <v>90</v>
       </c>
       <c r="N145" s="193">
-        <f t="shared" si="94"/>
-        <v>50</v>
+        <f t="shared" si="102"/>
+        <v>30</v>
       </c>
       <c r="O145" s="194">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>20</v>
       </c>
     </row>
@@ -12839,44 +12836,44 @@
         <v>50</v>
       </c>
       <c r="F147" s="70">
-        <f t="shared" ref="F147:O147" si="95">E147+F149-F145</f>
+        <f t="shared" ref="F147:O147" si="103">E147+F149-F145</f>
         <v>30</v>
       </c>
       <c r="G147" s="70">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>50</v>
       </c>
       <c r="H147" s="70">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>30</v>
       </c>
       <c r="I147" s="70">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>60</v>
       </c>
       <c r="J147" s="70">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
+        <v>50</v>
+      </c>
+      <c r="K147" s="70">
+        <f t="shared" si="103"/>
         <v>30</v>
       </c>
-      <c r="K147" s="70">
-        <f t="shared" si="95"/>
-        <v>30</v>
-      </c>
       <c r="L147" s="70">
-        <f t="shared" si="95"/>
-        <v>30</v>
+        <f t="shared" si="103"/>
+        <v>60</v>
       </c>
       <c r="M147" s="70">
-        <f t="shared" si="95"/>
-        <v>60</v>
+        <f t="shared" si="103"/>
+        <v>70</v>
       </c>
       <c r="N147" s="70">
-        <f t="shared" si="95"/>
-        <v>60</v>
+        <f t="shared" si="103"/>
+        <v>40</v>
       </c>
       <c r="O147" s="71">
-        <f t="shared" si="95"/>
-        <v>40</v>
+        <f t="shared" si="103"/>
+        <v>70</v>
       </c>
     </row>
     <row r="148" spans="3:16" x14ac:dyDescent="0.3">
@@ -12885,44 +12882,44 @@
       </c>
       <c r="E148" s="73"/>
       <c r="F148" s="70">
-        <f t="shared" ref="F148:O148" si="96">IF(E147-F145&lt;=$E$142, F145-E147+$E$142,0)</f>
+        <f t="shared" ref="F148:O148" si="104">IF(E147-F145&lt;=$E$142, F145-E147+$E$142,0)</f>
         <v>0</v>
       </c>
       <c r="G148" s="70">
-        <f t="shared" si="96"/>
+        <f t="shared" si="104"/>
         <v>80</v>
       </c>
       <c r="H148" s="70">
-        <f t="shared" si="96"/>
+        <f t="shared" si="104"/>
         <v>200</v>
       </c>
       <c r="I148" s="70">
-        <f t="shared" si="96"/>
+        <f t="shared" si="104"/>
         <v>170</v>
       </c>
       <c r="J148" s="70">
-        <f t="shared" si="96"/>
+        <f t="shared" si="104"/>
+        <v>230</v>
+      </c>
+      <c r="K148" s="70">
+        <f t="shared" si="104"/>
         <v>200</v>
       </c>
-      <c r="K148" s="70">
-        <f t="shared" si="96"/>
-        <v>200</v>
-      </c>
       <c r="L148" s="70">
-        <f t="shared" si="96"/>
-        <v>200</v>
+        <f t="shared" si="104"/>
+        <v>220</v>
       </c>
       <c r="M148" s="70">
-        <f t="shared" si="96"/>
-        <v>70</v>
+        <f t="shared" si="104"/>
+        <v>60</v>
       </c>
       <c r="N148" s="70">
-        <f t="shared" si="96"/>
-        <v>20</v>
+        <f t="shared" si="104"/>
+        <v>0</v>
       </c>
       <c r="O148" s="71">
-        <f t="shared" si="96"/>
-        <v>0</v>
+        <f t="shared" si="104"/>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="3:16" x14ac:dyDescent="0.3">
@@ -12935,40 +12932,40 @@
         <v>0</v>
       </c>
       <c r="G149" s="70">
-        <f t="shared" ref="G149:O149" si="97" xml:space="preserve"> CEILING(G148/$E$141,1)*$E$141</f>
+        <f t="shared" ref="G149:O149" si="105" xml:space="preserve"> CEILING(G148/$E$141,1)*$E$141</f>
         <v>100</v>
       </c>
       <c r="H149" s="199">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>200</v>
       </c>
       <c r="I149" s="70">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>200</v>
       </c>
       <c r="J149" s="70">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
+        <v>250</v>
+      </c>
+      <c r="K149" s="70">
+        <f t="shared" si="105"/>
         <v>200</v>
       </c>
-      <c r="K149" s="70">
-        <f t="shared" si="97"/>
-        <v>200</v>
-      </c>
       <c r="L149" s="70">
-        <f t="shared" si="97"/>
-        <v>200</v>
+        <f t="shared" si="105"/>
+        <v>250</v>
       </c>
       <c r="M149" s="70">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>100</v>
       </c>
       <c r="N149" s="70">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
+        <v>0</v>
+      </c>
+      <c r="O149" s="71">
+        <f t="shared" si="105"/>
         <v>50</v>
-      </c>
-      <c r="O149" s="71">
-        <f t="shared" si="97"/>
-        <v>0</v>
       </c>
     </row>
     <row r="150" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -12985,35 +12982,35 @@
         <v>200</v>
       </c>
       <c r="H150" s="202">
-        <f t="shared" ref="H150:O150" si="98">I149</f>
+        <f t="shared" ref="H150:O150" si="106">I149</f>
         <v>200</v>
       </c>
       <c r="I150" s="202">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
+        <v>250</v>
+      </c>
+      <c r="J150" s="202">
+        <f t="shared" si="106"/>
         <v>200</v>
       </c>
-      <c r="J150" s="202">
-        <f t="shared" si="98"/>
-        <v>200</v>
-      </c>
       <c r="K150" s="202">
-        <f t="shared" si="98"/>
-        <v>200</v>
+        <f t="shared" si="106"/>
+        <v>250</v>
       </c>
       <c r="L150" s="202">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>100</v>
       </c>
       <c r="M150" s="202">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
+        <v>0</v>
+      </c>
+      <c r="N150" s="202">
+        <f t="shared" si="106"/>
         <v>50</v>
       </c>
-      <c r="N150" s="202">
-        <f t="shared" si="98"/>
-        <v>0</v>
-      </c>
       <c r="O150" s="203">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0</v>
       </c>
       <c r="P150" s="134"/>
@@ -13028,7 +13025,7 @@
         <v>0</v>
       </c>
       <c r="G151" s="206">
-        <f t="shared" ref="G151:O152" si="99">IF(G148&gt;$E$143,G148-$E$143,0)</f>
+        <f t="shared" ref="G151:O152" si="107">IF(G148&gt;$E$143,G148-$E$143,0)</f>
         <v>0</v>
       </c>
       <c r="H151" s="206">
@@ -13036,31 +13033,31 @@
         <v>0</v>
       </c>
       <c r="I151" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="J151" s="206">
-        <f t="shared" si="99"/>
-        <v>0</v>
+        <f t="shared" si="107"/>
+        <v>30</v>
       </c>
       <c r="K151" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="L151" s="206">
-        <f t="shared" si="99"/>
-        <v>0</v>
+        <f t="shared" si="107"/>
+        <v>20</v>
       </c>
       <c r="M151" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="N151" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="O151" s="207">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="P151" s="134"/>
@@ -13075,7 +13072,7 @@
         <v>0</v>
       </c>
       <c r="G152" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="H152" s="206">
@@ -13083,31 +13080,31 @@
         <v>0</v>
       </c>
       <c r="I152" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="J152" s="206">
-        <f t="shared" si="99"/>
-        <v>0</v>
+        <f t="shared" si="107"/>
+        <v>50</v>
       </c>
       <c r="K152" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="L152" s="206">
-        <f t="shared" si="99"/>
-        <v>0</v>
+        <f t="shared" si="107"/>
+        <v>50</v>
       </c>
       <c r="M152" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="N152" s="206">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="O152" s="207">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
       <c r="P152" s="134"/>

</xml_diff>

<commit_message>
Final tested drp for 1 supplier - nonclass
</commit_message>
<xml_diff>
--- a/DRP/demand_data.xlsx
+++ b/DRP/demand_data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721D8632-7A78-4827-AD88-768A4F03CABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37342DF2-CFBC-4A1F-BDF8-7328ECCF2954}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21375" yWindow="2355" windowWidth="17280" windowHeight="8970" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC1" sheetId="1" r:id="rId1"/>
     <sheet name="DC2" sheetId="2" r:id="rId2"/>
     <sheet name="DC3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sup" sheetId="4" r:id="rId4"/>
+    <sheet name="Supplier1" sheetId="4" r:id="rId4"/>
     <sheet name="Selection" sheetId="5" r:id="rId5"/>
     <sheet name="DRP simulation" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId7"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="138">
   <si>
     <t>W46</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Lead Time (weeks)</t>
-  </si>
-  <si>
     <t>Lot Size (MT)</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
   </si>
   <si>
     <t>Price</t>
-  </si>
-  <si>
-    <t>Max Daily Production</t>
   </si>
   <si>
     <t>Method</t>
@@ -521,6 +515,24 @@
   </si>
   <si>
     <t>SDTR (accum)</t>
+  </si>
+  <si>
+    <t>Delivery Lead Time (weeks) - sup 1</t>
+  </si>
+  <si>
+    <t>Delivery Lead Time (weeks) - sup 2</t>
+  </si>
+  <si>
+    <t>Max Weekly Production</t>
+  </si>
+  <si>
+    <t>Production Lead Time (weeks)</t>
+  </si>
+  <si>
+    <t>Prebuild Inventory</t>
+  </si>
+  <si>
+    <t>Reduce Demand</t>
   </si>
 </sst>
 </file>
@@ -3872,7 +3884,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3883,7 +3895,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3894,12 +3906,12 @@
         <v>19</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="242" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="235">
         <v>20</v>
@@ -3908,13 +3920,13 @@
         <v>600</v>
       </c>
       <c r="F3" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H3" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -3924,7 +3936,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="243" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="236">
         <v>10</v>
@@ -3933,13 +3945,13 @@
         <v>350</v>
       </c>
       <c r="F4" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H4" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -3949,7 +3961,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="242" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="235">
         <v>20</v>
@@ -3958,13 +3970,13 @@
         <v>500</v>
       </c>
       <c r="F5" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H5" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -3974,7 +3986,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="243" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="236">
         <v>10</v>
@@ -3983,13 +3995,13 @@
         <v>280</v>
       </c>
       <c r="F6" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H6" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -3999,20 +4011,20 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="243" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C7" s="237">
         <v>2</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H7" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -4022,20 +4034,20 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="243" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C8" s="237">
         <v>1</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H8" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -4045,7 +4057,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="243" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="238">
         <v>10</v>
@@ -4062,7 +4074,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="244" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="239">
         <v>30</v>
@@ -4310,7 +4322,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4321,7 +4333,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4332,12 +4344,12 @@
         <v>19</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="242" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="236">
         <v>20</v>
@@ -4346,13 +4358,13 @@
         <v>500</v>
       </c>
       <c r="F3" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H3" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -4362,7 +4374,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="243" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="236">
         <v>10</v>
@@ -4371,13 +4383,13 @@
         <v>280</v>
       </c>
       <c r="F4" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H4" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -4387,7 +4399,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="242" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="236">
         <v>20</v>
@@ -4396,13 +4408,13 @@
         <v>480</v>
       </c>
       <c r="F5" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H5" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -4412,7 +4424,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="243" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="236">
         <v>10</v>
@@ -4421,13 +4433,13 @@
         <v>250</v>
       </c>
       <c r="F6" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H6" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -4437,20 +4449,20 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="243" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C7" s="237">
         <v>1</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H7" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -4460,20 +4472,20 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="243" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C8" s="237">
         <v>1</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H8" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -4483,7 +4495,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="243" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="239">
         <v>20</v>
@@ -4500,7 +4512,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="244" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="239">
         <v>20</v>
@@ -4740,7 +4752,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4751,7 +4763,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4762,12 +4774,12 @@
         <v>19</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" s="242" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="236">
         <v>20</v>
@@ -4776,13 +4788,13 @@
         <v>200</v>
       </c>
       <c r="F3" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H3" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -4792,7 +4804,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" s="243" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" s="236">
         <v>10</v>
@@ -4801,13 +4813,13 @@
         <v>120</v>
       </c>
       <c r="F4" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G4" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H4" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -4817,7 +4829,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" s="242" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C5" s="236">
         <v>20</v>
@@ -4826,13 +4838,13 @@
         <v>400</v>
       </c>
       <c r="F5" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H5" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H5" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -4842,7 +4854,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" s="243" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C6" s="236">
         <v>10</v>
@@ -4851,13 +4863,13 @@
         <v>250</v>
       </c>
       <c r="F6" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H6" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -4867,20 +4879,20 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" s="243" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C7" s="237">
         <v>0</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="262" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="263" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="262" t="s">
         <v>119</v>
-      </c>
-      <c r="H7" s="262" t="s">
-        <v>121</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -4890,20 +4902,20 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" s="243" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C8" s="237">
         <v>1</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="260" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="261" t="s">
+        <v>118</v>
+      </c>
+      <c r="H8" s="260" t="s">
         <v>120</v>
-      </c>
-      <c r="H8" s="260" t="s">
-        <v>122</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -4913,7 +4925,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" s="243" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="239">
         <v>10</v>
@@ -4930,7 +4942,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10" s="244" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="239">
         <v>10</v>
@@ -5176,7 +5188,7 @@
   <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5204,7 +5216,7 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="38" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="C4" s="44">
         <v>200</v>
@@ -5220,17 +5232,17 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="C5" s="40">
         <v>1</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -5241,7 +5253,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="45">
         <v>50</v>
@@ -5258,7 +5270,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="45">
         <v>30</v>
@@ -5281,29 +5293,29 @@
         <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="49" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="49" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
       <c r="H9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5329,19 +5341,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -5353,8 +5365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B409AB02-E9CA-40CB-B386-70D450CE0A6B}">
   <dimension ref="A2:AH209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D108" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M140" sqref="M140"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5380,7 +5392,7 @@
       <c r="A2" s="50"/>
       <c r="B2" s="50"/>
       <c r="D2" s="51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -5388,23 +5400,23 @@
       <c r="B3" s="50"/>
       <c r="D3" s="51"/>
       <c r="J3" s="50" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C4" s="52" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="50" t="s">
         <v>36</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="50" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E5" s="238">
         <f>'DC1'!C3</f>
@@ -5419,7 +5431,7 @@
     </row>
     <row r="6" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E6" s="238">
         <f>'DC1'!C4</f>
@@ -5434,7 +5446,7 @@
     </row>
     <row r="7" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="266" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E7" s="267">
         <f>'DC1'!C5</f>
@@ -5450,7 +5462,7 @@
     </row>
     <row r="8" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="266" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E8" s="267">
         <f>'DC1'!C6</f>
@@ -5466,14 +5478,14 @@
     </row>
     <row r="9" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E9" s="238">
         <f>'DC1'!C7</f>
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O9" s="280">
         <v>1</v>
@@ -5481,50 +5493,50 @@
     </row>
     <row r="10" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="266" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E10" s="267">
         <f>'DC1'!C8</f>
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O10" s="280"/>
     </row>
     <row r="11" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E11" s="6">
         <f>'DC1'!C9</f>
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11" s="265"/>
       <c r="K11" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O11" s="280"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="7">
         <f>'DC1'!C10</f>
         <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O12" s="281"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E13" s="253" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F13" s="254" t="s">
         <v>0</v>
@@ -5557,7 +5569,7 @@
         <v>9</v>
       </c>
       <c r="P13" s="56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -5606,12 +5618,12 @@
         <v>10</v>
       </c>
       <c r="P14" s="58" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15" s="50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>11</v>
@@ -5706,7 +5718,7 @@
     </row>
     <row r="17" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C17" s="50" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>13</v>
@@ -5755,7 +5767,7 @@
     </row>
     <row r="18" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D18" s="61" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" s="62"/>
       <c r="F18" s="63">
@@ -5821,12 +5833,12 @@
       <c r="N19" s="248"/>
       <c r="O19" s="249"/>
       <c r="P19" s="50" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="3:30" x14ac:dyDescent="0.3">
       <c r="D20" s="68" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" s="69">
         <f>'DC1'!C11</f>
@@ -5873,15 +5885,15 @@
         <v>35</v>
       </c>
       <c r="Q20" s="72" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C21" s="50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D21" s="68" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E21" s="73"/>
       <c r="F21" s="70">
@@ -5925,12 +5937,12 @@
         <v>5</v>
       </c>
       <c r="Q21" s="72" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="3:30" x14ac:dyDescent="0.3">
       <c r="D22" s="74" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" s="73"/>
       <c r="F22" s="70"/>
@@ -5970,7 +5982,7 @@
     </row>
     <row r="23" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="75" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="76"/>
       <c r="F23" s="77">
@@ -6016,7 +6028,7 @@
     </row>
     <row r="24" spans="3:30" x14ac:dyDescent="0.3">
       <c r="D24" s="79" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E24" s="80"/>
       <c r="F24" s="81">
@@ -6063,7 +6075,7 @@
     <row r="25" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C25" s="50"/>
       <c r="D25" s="83" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E25" s="84"/>
       <c r="F25" s="85">
@@ -6109,7 +6121,7 @@
     </row>
     <row r="26" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="87" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E26" s="88"/>
       <c r="F26" s="89">
@@ -6201,10 +6213,10 @@
     </row>
     <row r="28" spans="3:30" x14ac:dyDescent="0.3">
       <c r="C28" s="50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D28" s="95" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E28" s="96"/>
       <c r="F28" s="97">
@@ -6248,7 +6260,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AD28">
         <v>10</v>
@@ -6256,7 +6268,7 @@
     </row>
     <row r="29" spans="3:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D29" s="100" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E29" s="101"/>
       <c r="F29" s="102">
@@ -6300,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AD29">
         <v>20</v>
@@ -6354,7 +6366,7 @@
     </row>
     <row r="31" spans="3:30" x14ac:dyDescent="0.3">
       <c r="D31" s="95" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E31" s="105"/>
       <c r="F31" s="106">
@@ -6398,12 +6410,12 @@
         <v>0</v>
       </c>
       <c r="P31" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="3:30" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D32" s="108" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E32" s="109"/>
       <c r="F32" s="110">
@@ -6447,12 +6459,12 @@
         <v>0</v>
       </c>
       <c r="P32" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D33" s="79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E33" s="112"/>
       <c r="F33" s="81">
@@ -6496,22 +6508,22 @@
         <v>0</v>
       </c>
       <c r="P33" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AC33" s="113" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AD33" s="114"/>
       <c r="AF33" s="115" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AH33" s="115" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D34" s="116" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E34" s="112"/>
       <c r="F34" s="81">
@@ -6562,7 +6574,7 @@
     </row>
     <row r="35" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D35" s="278" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E35" s="273"/>
       <c r="F35" s="274">
@@ -6570,7 +6582,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="274">
-        <f t="shared" ref="G35:O35" si="15">MIN(MAX(G$151-(I22-I21),0),G33)</f>
+        <f t="shared" ref="G35:N35" si="15">MIN(MAX(G$151-(I22-I21),0),G33)</f>
         <v>0</v>
       </c>
       <c r="H35" s="274">
@@ -6612,7 +6624,7 @@
     </row>
     <row r="36" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D36" s="119" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E36" s="84"/>
       <c r="F36" s="85">
@@ -6656,36 +6668,36 @@
         <v>0</v>
       </c>
       <c r="P36" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA36" s="120" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB36" s="120" t="s">
         <v>74</v>
       </c>
-      <c r="AA36" s="120" t="s">
+      <c r="AC36" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="AB36" s="120" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC36" s="121" t="s">
-        <v>77</v>
-      </c>
       <c r="AD36" s="122" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AE36" s="118" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AF36" s="123" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG36" s="118" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="AH36" s="124" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D37" s="125" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="84"/>
       <c r="F37" s="85">
@@ -6779,7 +6791,7 @@
     </row>
     <row r="38" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D38" s="130" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E38" s="131"/>
       <c r="F38" s="132">
@@ -6873,10 +6885,10 @@
     </row>
     <row r="39" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C39" s="50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D39" s="135" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E39" s="92"/>
       <c r="F39" s="140">
@@ -6971,7 +6983,7 @@
     <row r="40" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="50"/>
       <c r="D40" s="137" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E40" s="138"/>
       <c r="F40" s="110">
@@ -7065,7 +7077,7 @@
     </row>
     <row r="41" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D41" s="139" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E41" s="92"/>
       <c r="F41" s="140">
@@ -7159,7 +7171,7 @@
     </row>
     <row r="42" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D42" s="137" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E42" s="142"/>
       <c r="F42" s="143">
@@ -7203,7 +7215,7 @@
         <v>0</v>
       </c>
       <c r="P42" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="V42">
         <f t="shared" si="19"/>
@@ -7255,7 +7267,7 @@
     </row>
     <row r="43" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D43" s="146" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E43" s="147"/>
       <c r="F43" s="148">
@@ -7348,7 +7360,7 @@
     </row>
     <row r="44" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D44" s="150" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E44" s="151"/>
       <c r="F44" s="152" t="e">
@@ -7441,7 +7453,7 @@
     </row>
     <row r="45" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D45" s="150" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E45" s="151"/>
       <c r="F45" s="152" t="e">
@@ -7534,7 +7546,7 @@
     </row>
     <row r="46" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D46" s="150" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E46" s="153"/>
       <c r="F46" s="152" t="e">
@@ -7677,10 +7689,10 @@
     </row>
     <row r="48" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C48" s="52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D48" s="53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E48" s="4"/>
       <c r="V48">
@@ -7733,7 +7745,7 @@
     </row>
     <row r="49" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D49" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E49" s="2">
         <f>'DC2'!C3</f>
@@ -7745,7 +7757,7 @@
       </c>
       <c r="G49"/>
       <c r="I49" s="72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P49" s="4"/>
       <c r="V49">
@@ -7798,7 +7810,7 @@
     </row>
     <row r="50" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D50" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E50" s="2">
         <f>'DC2'!C4</f>
@@ -7861,7 +7873,7 @@
     </row>
     <row r="51" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D51" s="266" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E51" s="269">
         <f>'DC2'!C5</f>
@@ -7888,7 +7900,7 @@
     </row>
     <row r="52" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D52" s="266" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E52" s="269">
         <f>'DC2'!C6</f>
@@ -7914,14 +7926,14 @@
     </row>
     <row r="53" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E53" s="5">
         <f>'DC2'!C7</f>
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O53" s="280">
         <v>2</v>
@@ -7979,14 +7991,14 @@
     </row>
     <row r="54" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="266" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E54" s="271">
         <f>'DC2'!C8</f>
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O54" s="280"/>
       <c r="Q54">
@@ -8002,17 +8014,17 @@
     </row>
     <row r="55" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D55" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E55" s="7">
         <f>'DC2'!C9</f>
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K55" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O55" s="280"/>
       <c r="V55">
@@ -8065,14 +8077,14 @@
     </row>
     <row r="56" spans="3:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D56" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E56" s="7">
         <f>'DC2'!C10</f>
         <v>20</v>
       </c>
       <c r="F56" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O56" s="281"/>
       <c r="V56">
@@ -8126,7 +8138,7 @@
     <row r="57" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C57" s="154"/>
       <c r="E57" s="253" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F57" s="254" t="s">
         <v>0</v>
@@ -8580,7 +8592,7 @@
     </row>
     <row r="62" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D62" s="61" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E62" s="62"/>
       <c r="F62" s="63">
@@ -8742,7 +8754,7 @@
     </row>
     <row r="64" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D64" s="68" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E64" s="69">
         <f>'DC2'!C11</f>
@@ -8789,7 +8801,7 @@
         <v>25</v>
       </c>
       <c r="Q64" s="72" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V64">
         <f t="shared" si="19"/>
@@ -8841,10 +8853,10 @@
     </row>
     <row r="65" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C65" s="50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D65" s="68" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E65" s="73"/>
       <c r="F65" s="70">
@@ -8888,7 +8900,7 @@
         <v>0</v>
       </c>
       <c r="Q65" s="72" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="V65">
         <f t="shared" si="19"/>
@@ -8940,7 +8952,7 @@
     </row>
     <row r="66" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D66" s="74" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E66" s="73"/>
       <c r="F66" s="70">
@@ -9033,7 +9045,7 @@
     </row>
     <row r="67" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D67" s="75" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E67" s="76"/>
       <c r="F67" s="77">
@@ -9122,7 +9134,7 @@
     </row>
     <row r="68" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D68" s="79" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E68" s="80"/>
       <c r="F68" s="81">
@@ -9212,7 +9224,7 @@
     <row r="69" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C69" s="50"/>
       <c r="D69" s="83" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E69" s="155"/>
       <c r="F69" s="85">
@@ -9301,7 +9313,7 @@
     </row>
     <row r="70" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D70" s="87" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E70" s="88"/>
       <c r="F70" s="89">
@@ -9479,10 +9491,10 @@
     </row>
     <row r="72" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C72" s="50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D72" s="157" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E72" s="96"/>
       <c r="F72" s="97">
@@ -9526,7 +9538,7 @@
         <v>0</v>
       </c>
       <c r="P72" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="W72">
         <v>32</v>
@@ -9574,7 +9586,7 @@
     </row>
     <row r="73" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D73" s="158" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E73" s="101"/>
       <c r="F73" s="102">
@@ -9618,7 +9630,7 @@
         <v>0</v>
       </c>
       <c r="P73" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="W73">
         <v>33</v>
@@ -9755,7 +9767,7 @@
     </row>
     <row r="75" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D75" s="95" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E75" s="105"/>
       <c r="F75" s="106">
@@ -9799,7 +9811,7 @@
         <v>0</v>
       </c>
       <c r="P75" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="W75">
         <v>35</v>
@@ -9847,7 +9859,7 @@
     </row>
     <row r="76" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D76" s="108" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E76" s="109"/>
       <c r="F76" s="110">
@@ -9891,7 +9903,7 @@
         <v>0</v>
       </c>
       <c r="P76" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="W76">
         <v>36</v>
@@ -9939,7 +9951,7 @@
     </row>
     <row r="77" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D77" s="159" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E77" s="222"/>
       <c r="F77" s="223">
@@ -9983,7 +9995,7 @@
         <v>0</v>
       </c>
       <c r="P77" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W77">
         <v>37</v>
@@ -10031,7 +10043,7 @@
     </row>
     <row r="78" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D78" s="116" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E78" s="112"/>
       <c r="F78" s="81">
@@ -10075,7 +10087,7 @@
         <v>0</v>
       </c>
       <c r="P78" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W78">
         <v>38</v>
@@ -10123,7 +10135,7 @@
     </row>
     <row r="79" spans="3:34" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D79" s="278" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E79" s="273"/>
       <c r="F79" s="274">
@@ -10174,7 +10186,7 @@
     </row>
     <row r="80" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D80" s="160" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E80" s="161"/>
       <c r="F80" s="85">
@@ -10264,7 +10276,7 @@
     </row>
     <row r="81" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D81" s="162" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E81" s="84"/>
       <c r="F81" s="85">
@@ -10354,7 +10366,7 @@
     </row>
     <row r="82" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D82" s="163" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E82" s="131"/>
       <c r="F82" s="132">
@@ -10444,10 +10456,10 @@
     </row>
     <row r="83" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C83" s="50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D83" s="135" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E83" s="92"/>
       <c r="F83" s="140">
@@ -10538,7 +10550,7 @@
     <row r="84" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C84" s="50"/>
       <c r="D84" s="137" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E84" s="138"/>
       <c r="F84" s="110">
@@ -10586,7 +10598,7 @@
     </row>
     <row r="85" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D85" s="139" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E85" s="92"/>
       <c r="F85" s="140">
@@ -10634,7 +10646,7 @@
     </row>
     <row r="86" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D86" s="137" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E86" s="142"/>
       <c r="F86" s="143">
@@ -10678,13 +10690,13 @@
         <v>0</v>
       </c>
       <c r="P86" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="AA86" s="169"/>
     </row>
     <row r="87" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D87" s="146" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E87" s="147"/>
       <c r="F87" s="148">
@@ -10731,7 +10743,7 @@
     </row>
     <row r="88" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D88" s="150" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E88" s="151"/>
       <c r="F88" s="152">
@@ -10778,7 +10790,7 @@
     </row>
     <row r="89" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D89" s="150" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E89" s="151"/>
       <c r="F89" s="152">
@@ -10825,7 +10837,7 @@
     </row>
     <row r="90" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D90" s="150" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E90" s="153"/>
       <c r="F90" s="152">
@@ -10891,17 +10903,17 @@
     </row>
     <row r="93" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C93" s="52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D93" s="53" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E93" s="4"/>
       <c r="AA93" s="169"/>
     </row>
     <row r="94" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D94" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E94" s="2">
         <f>'DC3'!C3</f>
@@ -10915,7 +10927,7 @@
     </row>
     <row r="95" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D95" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E95" s="2">
         <f>'DC3'!C4</f>
@@ -10930,7 +10942,7 @@
     </row>
     <row r="96" spans="3:34" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D96" s="266" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E96" s="269">
         <f>'DC3'!C5</f>
@@ -10945,7 +10957,7 @@
     </row>
     <row r="97" spans="4:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D97" s="266" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E97" s="269">
         <f>'DC3'!C6</f>
@@ -10960,14 +10972,14 @@
     </row>
     <row r="98" spans="4:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D98" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E98" s="5">
         <f>'DC3'!C7</f>
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O98" s="280">
         <v>3</v>
@@ -10976,50 +10988,50 @@
     </row>
     <row r="99" spans="4:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D99" s="266" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E99" s="271">
         <f>'DC3'!C8</f>
         <v>1</v>
       </c>
       <c r="F99" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O99" s="280"/>
       <c r="AA99" s="169"/>
     </row>
     <row r="100" spans="4:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D100" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E100" s="7">
         <f>'DC3'!C9</f>
         <v>10</v>
       </c>
       <c r="F100" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K100" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O100" s="280"/>
     </row>
     <row r="101" spans="4:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D101" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E101" s="7">
         <f>'DC3'!C10</f>
         <v>10</v>
       </c>
       <c r="F101" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O101" s="281"/>
     </row>
     <row r="102" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E102" s="55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F102" s="8" t="s">
         <v>0</v>
@@ -11238,7 +11250,7 @@
     </row>
     <row r="107" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D107" s="221" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E107" s="213"/>
       <c r="F107" s="214">
@@ -11306,7 +11318,7 @@
     </row>
     <row r="109" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D109" s="176" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E109" s="69">
         <f>'DC3'!C11</f>
@@ -11353,12 +11365,12 @@
         <v>15</v>
       </c>
       <c r="Q109" s="72" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="110" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D110" s="176" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E110" s="179"/>
       <c r="F110" s="177">
@@ -11402,12 +11414,12 @@
         <v>15</v>
       </c>
       <c r="Q110" s="72" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="111" spans="4:27" x14ac:dyDescent="0.3">
       <c r="D111" s="180" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E111" s="179"/>
       <c r="F111" s="177">
@@ -11453,7 +11465,7 @@
     </row>
     <row r="112" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D112" s="181" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E112" s="182"/>
       <c r="F112" s="183">
@@ -11499,7 +11511,7 @@
     </row>
     <row r="113" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D113" s="116" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E113" s="80"/>
       <c r="F113" s="81">
@@ -11546,7 +11558,7 @@
     <row r="114" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C114" s="50"/>
       <c r="D114" s="185" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E114" s="155"/>
       <c r="F114" s="85">
@@ -11592,7 +11604,7 @@
     </row>
     <row r="115" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D115" s="186" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E115" s="88"/>
       <c r="F115" s="89">
@@ -11684,10 +11696,10 @@
     </row>
     <row r="117" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C117" s="50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D117" s="95" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E117" s="96"/>
       <c r="F117" s="97">
@@ -11731,12 +11743,12 @@
         <v>4180</v>
       </c>
       <c r="P117" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="118" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D118" s="100" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E118" s="101"/>
       <c r="F118" s="102">
@@ -11780,7 +11792,7 @@
         <v>4380</v>
       </c>
       <c r="P118" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="119" spans="3:34" x14ac:dyDescent="0.3">
@@ -11831,7 +11843,7 @@
     </row>
     <row r="120" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D120" s="95" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E120" s="105"/>
       <c r="F120" s="106">
@@ -11875,12 +11887,12 @@
         <v>8440</v>
       </c>
       <c r="P120" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="121" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D121" s="108" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E121" s="109"/>
       <c r="F121" s="110">
@@ -11924,12 +11936,12 @@
         <v>4060</v>
       </c>
       <c r="P121" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="122" spans="3:34" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D122" s="159" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E122" s="222"/>
       <c r="F122" s="223">
@@ -11973,12 +11985,12 @@
         <v>0</v>
       </c>
       <c r="P122" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="123" spans="3:34" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D123" s="116" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E123" s="112"/>
       <c r="F123" s="81">
@@ -12022,7 +12034,7 @@
         <v>0</v>
       </c>
       <c r="P123" s="50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="W123">
         <v>38</v>
@@ -12070,7 +12082,7 @@
     </row>
     <row r="124" spans="3:34" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D124" s="278" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E124" s="273"/>
       <c r="F124" s="274">
@@ -12123,7 +12135,7 @@
     </row>
     <row r="125" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D125" s="160" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E125" s="161"/>
       <c r="F125" s="85">
@@ -12170,7 +12182,7 @@
     </row>
     <row r="126" spans="3:34" x14ac:dyDescent="0.3">
       <c r="D126" s="162" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E126" s="84"/>
       <c r="F126" s="85">
@@ -12217,7 +12229,7 @@
     </row>
     <row r="127" spans="3:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D127" s="163" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E127" s="131"/>
       <c r="F127" s="132">
@@ -12264,10 +12276,10 @@
     </row>
     <row r="128" spans="3:34" x14ac:dyDescent="0.3">
       <c r="C128" s="50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D128" s="135" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E128" s="92"/>
       <c r="F128" s="140">
@@ -12315,7 +12327,7 @@
     <row r="129" spans="3:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C129" s="50"/>
       <c r="D129" s="137" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E129" s="138"/>
       <c r="F129" s="110">
@@ -12362,7 +12374,7 @@
     </row>
     <row r="130" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D130" s="139" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E130" s="92"/>
       <c r="F130" s="140">
@@ -12409,7 +12421,7 @@
     </row>
     <row r="131" spans="3:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D131" s="137" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E131" s="142"/>
       <c r="F131" s="143">
@@ -12453,12 +12465,12 @@
         <v>0</v>
       </c>
       <c r="P131" s="50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="3:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D132" s="146" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E132" s="147"/>
       <c r="F132" s="148">
@@ -12505,7 +12517,7 @@
     </row>
     <row r="133" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D133" s="150" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E133" s="151"/>
       <c r="F133" s="152" t="e">
@@ -12552,7 +12564,7 @@
     </row>
     <row r="134" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D134" s="150" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E134" s="151"/>
       <c r="F134" s="152" t="e">
@@ -12599,7 +12611,7 @@
     </row>
     <row r="135" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D135" s="150" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E135" s="153"/>
       <c r="F135" s="152" t="e">
@@ -12674,65 +12686,65 @@
     </row>
     <row r="139" spans="3:27" x14ac:dyDescent="0.3">
       <c r="C139" s="188" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D139" s="189" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E139" s="190"/>
       <c r="F139" s="188"/>
     </row>
     <row r="140" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D140" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E140" s="5">
-        <f>Sup!C5</f>
+        <f>Supplier1!C5</f>
         <v>1</v>
       </c>
       <c r="F140" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="141" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D141" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E141" s="6">
-        <f>Sup!C6</f>
+        <f>Supplier1!C6</f>
         <v>50</v>
       </c>
       <c r="F141" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K141" s="54" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="142" spans="3:27" x14ac:dyDescent="0.3">
       <c r="D142" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E142" s="6">
-        <f>Sup!C7</f>
+        <f>Supplier1!C7</f>
         <v>30</v>
       </c>
       <c r="F142" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="143" spans="3:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D143" s="1" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="E143" s="7">
-        <f>Sup!C4</f>
+        <f>Supplier1!C4</f>
         <v>200</v>
       </c>
     </row>
     <row r="144" spans="3:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E144" s="55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F144" s="8" t="s">
         <v>0</v>
@@ -12741,7 +12753,7 @@
         <v>1</v>
       </c>
       <c r="H144" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I144" s="8" t="s">
         <v>3</v>
@@ -12767,7 +12779,7 @@
     </row>
     <row r="145" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D145" s="191" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E145" s="192"/>
       <c r="F145" s="193">
@@ -12813,7 +12825,7 @@
     </row>
     <row r="146" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D146" s="195" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E146" s="196"/>
       <c r="F146" s="197"/>
@@ -12829,10 +12841,10 @@
     </row>
     <row r="147" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D147" s="176" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E147" s="36">
-        <f>Sup!C8</f>
+        <f>Supplier1!C8</f>
         <v>50</v>
       </c>
       <c r="F147" s="70">
@@ -12878,7 +12890,7 @@
     </row>
     <row r="148" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D148" s="176" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E148" s="73"/>
       <c r="F148" s="70">
@@ -12924,7 +12936,7 @@
     </row>
     <row r="149" spans="3:16" x14ac:dyDescent="0.3">
       <c r="D149" s="180" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E149" s="73"/>
       <c r="F149" s="70">
@@ -12970,7 +12982,7 @@
     </row>
     <row r="150" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D150" s="200" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E150" s="201"/>
       <c r="F150" s="202">
@@ -13017,7 +13029,7 @@
     </row>
     <row r="151" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D151" s="204" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E151" s="205"/>
       <c r="F151" s="206">
@@ -13064,7 +13076,7 @@
     </row>
     <row r="152" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D152" s="204" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E152" s="205"/>
       <c r="F152" s="206">
@@ -13126,59 +13138,59 @@
     </row>
     <row r="156" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C156" s="49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H156" s="211" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="157" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C157" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H157" s="49" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="158" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C158" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="159" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C159" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="160" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C160" s="212" t="s">
+        <v>111</v>
+      </c>
+      <c r="D160" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="H160" s="211" t="s">
         <v>113</v>
-      </c>
-      <c r="D160" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="H160" s="211" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="161" spans="3:8" x14ac:dyDescent="0.3">
       <c r="H161" s="49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="163" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C163" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C186" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="209" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C209" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel file demand data
</commit_message>
<xml_diff>
--- a/DRP/demand_data.xlsx
+++ b/DRP/demand_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\ghub_acceval\smarttradzt-python-services\DRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C28CB12-25DB-45D1-B7FD-C99ACB48C34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25708DF-5BC6-447A-B5AC-F3EDA2956E62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2952" yWindow="708" windowWidth="18576" windowHeight="11580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC1" sheetId="1" r:id="rId1"/>
@@ -2471,14 +2471,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -3995,7 +3995,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:L16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4277,16 +4277,16 @@
       <c r="C14" s="230">
         <v>40</v>
       </c>
-      <c r="D14" s="281">
+      <c r="D14" s="279">
         <v>30</v>
       </c>
-      <c r="E14" s="281"/>
-      <c r="F14" s="281"/>
-      <c r="G14" s="281"/>
-      <c r="H14" s="281"/>
-      <c r="I14" s="281"/>
-      <c r="J14" s="281"/>
-      <c r="K14" s="281"/>
+      <c r="E14" s="279"/>
+      <c r="F14" s="279"/>
+      <c r="G14" s="279"/>
+      <c r="H14" s="279"/>
+      <c r="I14" s="279"/>
+      <c r="J14" s="279"/>
+      <c r="K14" s="279"/>
       <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -4294,22 +4294,22 @@
         <v>12</v>
       </c>
       <c r="C15" s="230"/>
-      <c r="D15" s="281"/>
-      <c r="E15" s="281">
+      <c r="D15" s="279"/>
+      <c r="E15" s="279">
         <v>20</v>
       </c>
-      <c r="F15" s="281">
+      <c r="F15" s="279">
         <v>50</v>
       </c>
-      <c r="G15" s="281">
+      <c r="G15" s="279">
         <v>60</v>
       </c>
-      <c r="H15" s="281"/>
-      <c r="I15" s="281">
+      <c r="H15" s="279"/>
+      <c r="I15" s="279">
         <v>40</v>
       </c>
-      <c r="J15" s="281"/>
-      <c r="K15" s="281">
+      <c r="J15" s="279"/>
+      <c r="K15" s="279">
         <v>40</v>
       </c>
       <c r="L15" s="15"/>
@@ -4321,16 +4321,16 @@
       <c r="C16" s="230">
         <v>50</v>
       </c>
-      <c r="D16" s="281">
+      <c r="D16" s="279">
         <v>40</v>
       </c>
-      <c r="E16" s="281"/>
-      <c r="F16" s="281"/>
-      <c r="G16" s="281"/>
-      <c r="H16" s="281"/>
-      <c r="I16" s="281"/>
-      <c r="J16" s="281"/>
-      <c r="K16" s="281"/>
+      <c r="E16" s="279"/>
+      <c r="F16" s="279"/>
+      <c r="G16" s="279"/>
+      <c r="H16" s="279"/>
+      <c r="I16" s="279"/>
+      <c r="J16" s="279"/>
+      <c r="K16" s="279"/>
       <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4713,16 +4713,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="230"/>
-      <c r="D14" s="281">
+      <c r="D14" s="279">
         <v>10</v>
       </c>
-      <c r="E14" s="281"/>
-      <c r="F14" s="281"/>
-      <c r="G14" s="281"/>
-      <c r="H14" s="281"/>
-      <c r="I14" s="281"/>
-      <c r="J14" s="281"/>
-      <c r="K14" s="281"/>
+      <c r="E14" s="279"/>
+      <c r="F14" s="279"/>
+      <c r="G14" s="279"/>
+      <c r="H14" s="279"/>
+      <c r="I14" s="279"/>
+      <c r="J14" s="279"/>
+      <c r="K14" s="279"/>
       <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -4730,20 +4730,20 @@
         <v>12</v>
       </c>
       <c r="C15" s="230"/>
-      <c r="D15" s="281"/>
-      <c r="E15" s="281"/>
-      <c r="F15" s="281">
+      <c r="D15" s="279"/>
+      <c r="E15" s="279"/>
+      <c r="F15" s="279">
         <v>60</v>
       </c>
-      <c r="G15" s="281">
+      <c r="G15" s="279">
         <v>80</v>
       </c>
-      <c r="H15" s="281"/>
-      <c r="I15" s="281">
+      <c r="H15" s="279"/>
+      <c r="I15" s="279">
         <v>40</v>
       </c>
-      <c r="J15" s="281"/>
-      <c r="K15" s="281">
+      <c r="J15" s="279"/>
+      <c r="K15" s="279">
         <v>50</v>
       </c>
       <c r="L15" s="15"/>
@@ -5487,8 +5487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B409AB02-E9CA-40CB-B386-70D450CE0A6B}">
   <dimension ref="A2:AH209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5609,7 +5609,7 @@
       <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="279">
+      <c r="O9" s="280">
         <v>1</v>
       </c>
     </row>
@@ -5624,7 +5624,7 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="279"/>
+      <c r="O10" s="280"/>
     </row>
     <row r="11" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
@@ -5641,7 +5641,7 @@
       <c r="K11" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="O11" s="279"/>
+      <c r="O11" s="280"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1" t="s">
@@ -5654,7 +5654,7 @@
       <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="O12" s="280"/>
+      <c r="O12" s="281"/>
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E13" s="252" t="s">
@@ -8057,7 +8057,7 @@
       <c r="F53" t="s">
         <v>34</v>
       </c>
-      <c r="O53" s="279">
+      <c r="O53" s="280">
         <v>2</v>
       </c>
       <c r="Q53">
@@ -8122,7 +8122,7 @@
       <c r="F54" t="s">
         <v>34</v>
       </c>
-      <c r="O54" s="279"/>
+      <c r="O54" s="280"/>
       <c r="Q54">
         <f>Q53+Q52</f>
         <v>442600</v>
@@ -8148,7 +8148,7 @@
       <c r="K55" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="O55" s="279"/>
+      <c r="O55" s="280"/>
       <c r="V55">
         <f t="shared" si="20"/>
         <v>5</v>
@@ -8208,7 +8208,7 @@
       <c r="F56" t="s">
         <v>35</v>
       </c>
-      <c r="O56" s="280"/>
+      <c r="O56" s="281"/>
       <c r="V56">
         <f>MOD(W56,$AD$28)</f>
         <v>6</v>
@@ -11103,7 +11103,7 @@
       <c r="F98" t="s">
         <v>34</v>
       </c>
-      <c r="O98" s="279">
+      <c r="O98" s="280">
         <v>3</v>
       </c>
       <c r="AA98" s="168"/>
@@ -11119,7 +11119,7 @@
       <c r="F99" t="s">
         <v>34</v>
       </c>
-      <c r="O99" s="279"/>
+      <c r="O99" s="280"/>
       <c r="AA99" s="168"/>
     </row>
     <row r="100" spans="4:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -11136,7 +11136,7 @@
       <c r="K100" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="O100" s="279"/>
+      <c r="O100" s="280"/>
     </row>
     <row r="101" spans="4:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D101" s="1" t="s">
@@ -11149,7 +11149,7 @@
       <c r="F101" t="s">
         <v>35</v>
       </c>
-      <c r="O101" s="280"/>
+      <c r="O101" s="281"/>
     </row>
     <row r="102" spans="4:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E102" s="54" t="s">

</xml_diff>